<commit_message>
squire qoroth stuff, ivywatch
</commit_message>
<xml_diff>
--- a/adventures/ivywatch/working/monsters.xlsx
+++ b/adventures/ivywatch/working/monsters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gavin\Documents\drawsteel\_products\adventures\ivywatch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gavin\Documents\drawsteel\_products\adventures\ivywatch\working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99685436-D313-49F8-AED1-33BDD6756962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2375E84E-D82C-4AC8-91F2-5F00D747BA59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="840" windowWidth="20475" windowHeight="13170" activeTab="2" xr2:uid="{918A4370-6BD2-4549-B40B-132AC3F5AF22}"/>
+    <workbookView xWindow="1710" yWindow="930" windowWidth="20475" windowHeight="14100" activeTab="2" xr2:uid="{918A4370-6BD2-4549-B40B-132AC3F5AF22}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="123">
   <si>
     <t>[Name]</t>
   </si>
@@ -1928,6 +1928,192 @@
       </rPr>
       <t xml:space="preserve"> The target is destroyed. All toxic plants that are destroyed as a result of this ability explode. All creatures and objects within 1 burst of an exploding toxic plant take 3 fire damage.</t>
     </r>
+  </si>
+  <si>
+    <t>Squire Qoroth</t>
+  </si>
+  <si>
+    <t>Level 1 Harrier Retainer</t>
+  </si>
+  <si>
+    <t>Fey, Humanoid, Wode Elf</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Stamina </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>20</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Speed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 7</t>
+    </r>
+  </si>
+  <si>
+    <t>Masking Glamour</t>
+  </si>
+  <si>
+    <t>Qoroth immediately hides at the end of his turn while in cover or concealment, even if he is observed.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Thorned Fist </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(Action) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>u</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2d10 + 2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>u</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Signature</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Keywords</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Charge, Melee, Strike, Weapon</t>
+    </r>
+  </si>
+  <si>
+    <t>3 damage</t>
+  </si>
+  <si>
+    <t>5 damage</t>
+  </si>
+  <si>
+    <t>7 damage; grow a thornskin</t>
+  </si>
+  <si>
+    <t>Veil of Thorns</t>
+  </si>
+  <si>
+    <t>While Qoroth has a thornskin, whenever he takes damage from a melee ability, he can lose his thornskin to shift 2 and cause the attacker to bleed (save ends).</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Free Strike</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Might 0    Agility 2    Reason 0    Intuition 1    Presence 0 </t>
   </si>
 </sst>
 </file>
@@ -2118,7 +2304,7 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyBorder="1"/>
@@ -2141,21 +2327,39 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="9"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="10"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
@@ -2167,56 +2371,31 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="11" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="11" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="11" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="11" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -2566,16 +2745,16 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="28" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
       <c r="H1" s="8" t="s">
         <v>23</v>
       </c>
@@ -2587,10 +2766,10 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
-      <c r="P1" s="28" t="s">
+      <c r="P1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="28"/>
+      <c r="Q1" s="21"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="2" t="s">
@@ -2716,50 +2895,50 @@
       <c r="Q6" s="1"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
       <c r="H7" s="13" t="s">
         <v>29</v>
       </c>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
-      <c r="L7" s="29" t="s">
+      <c r="L7" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
       <c r="H8" s="14" t="s">
         <v>30</v>
       </c>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
-      <c r="L8" s="20" t="s">
+      <c r="L8" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="20"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="5" t="s">
@@ -2815,11 +2994,11 @@
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="H11" s="17" t="s">
         <v>33</v>
       </c>
@@ -2828,125 +3007,125 @@
       <c r="L11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="31"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
       <c r="L12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="31"/>
-      <c r="P12" s="31"/>
-      <c r="Q12" s="31"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
       <c r="L13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="31"/>
-      <c r="Q13" s="31"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="25"/>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="L14" s="18" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="L14" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
+      <c r="Q14" s="26"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="26"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
+      <c r="Q16" s="26"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="19"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="27"/>
     </row>
     <row r="18" spans="1:17">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="L18" s="20" t="s">
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="L18" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
-      <c r="O18" s="20"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="20"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="5" t="s">
@@ -2972,99 +3151,99 @@
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
       <c r="L20" s="5" t="s">
         <v>11</v>
       </c>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
-      <c r="O20" s="21" t="s">
+      <c r="O20" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="22"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="29"/>
     </row>
     <row r="21" spans="1:17">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="L21" s="23" t="s">
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="L21" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="M21" s="24"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="24"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="20"/>
     </row>
     <row r="22" spans="1:17">
-      <c r="A22" s="25"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="25"/>
-      <c r="O22" s="25"/>
-      <c r="P22" s="25"/>
-      <c r="Q22" s="25"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="31"/>
+      <c r="O22" s="31"/>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="31"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="L23" s="26" t="s">
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="L23" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="M23" s="27"/>
-      <c r="N23" s="27"/>
-      <c r="O23" s="27"/>
-      <c r="P23" s="27"/>
-      <c r="Q23" s="27"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="33"/>
+      <c r="O23" s="33"/>
+      <c r="P23" s="33"/>
+      <c r="Q23" s="33"/>
     </row>
     <row r="24" spans="1:17">
-      <c r="A24" s="24"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="24"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="24"/>
-      <c r="Q24" s="24"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="20"/>
+      <c r="P24" s="20"/>
+      <c r="Q24" s="20"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="24"/>
-      <c r="O25" s="24"/>
-      <c r="P25" s="24"/>
-      <c r="Q25" s="24"/>
+      <c r="A25" s="20"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="20"/>
+      <c r="O25" s="20"/>
+      <c r="P25" s="20"/>
+      <c r="Q25" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="25">
@@ -3113,10 +3292,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF82A8B5-C780-4855-A5A0-A052A5BEE04A}">
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3128,26 +3307,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="34" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="H1" s="44" t="s">
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="H1" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="45" t="s">
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
@@ -3179,7 +3358,7 @@
       <c r="C3" s="5"/>
       <c r="D3" s="1"/>
       <c r="E3" s="5"/>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="18" t="s">
         <v>59</v>
       </c>
       <c r="H3" s="5" t="s">
@@ -3189,7 +3368,7 @@
       <c r="J3" s="5"/>
       <c r="K3" s="1"/>
       <c r="L3" s="5"/>
-      <c r="M3" s="35"/>
+      <c r="M3" s="18"/>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="5" t="s">
@@ -3199,7 +3378,7 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="18" t="s">
         <v>40</v>
       </c>
       <c r="H4" s="5" t="s">
@@ -3209,7 +3388,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="5"/>
-      <c r="M4" s="35" t="s">
+      <c r="M4" s="18" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3219,7 +3398,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="18" t="s">
         <v>39</v>
       </c>
       <c r="H5" s="1"/>
@@ -3227,45 +3406,45 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="35" t="s">
+      <c r="M5" s="18" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="H6" s="29" t="s">
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="H6" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="H7" s="20" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="H7" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="5" t="s">
@@ -3291,119 +3470,119 @@
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
       <c r="H9" s="5" t="s">
         <v>87</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="41" t="s">
+      <c r="K9" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="H10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="37" t="s">
+      <c r="I10" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="H11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="37" t="s">
+      <c r="I11" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
       <c r="H12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="36" t="s">
+      <c r="I12" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="1"/>
-      <c r="B13" s="39"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
-      <c r="H13" s="46" t="s">
+      <c r="H13" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="46"/>
-      <c r="M13" s="46"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="5" t="s">
@@ -3414,14 +3593,14 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="5" t="s">
@@ -3429,11 +3608,11 @@
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="41" t="s">
+      <c r="D16" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
       <c r="H16" s="5" t="s">
         <v>50</v>
       </c>
@@ -3447,73 +3626,73 @@
       <c r="A17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
       <c r="H17" s="5" t="s">
         <v>87</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="41" t="s">
+      <c r="K17" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="L17" s="42"/>
-      <c r="M17" s="42"/>
+      <c r="L17" s="43"/>
+      <c r="M17" s="43"/>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="H18" s="23" t="s">
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="H18" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="H19" s="20" t="s">
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="H19" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
       <c r="H20" s="5" t="s">
         <v>50</v>
       </c>
@@ -3524,24 +3703,24 @@
       <c r="M20" s="1"/>
     </row>
     <row r="21" spans="1:13">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
       <c r="H21" s="5" t="s">
         <v>87</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
-      <c r="K21" s="41" t="s">
+      <c r="K21" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="L21" s="42"/>
-      <c r="M21" s="42"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="43"/>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="5" t="s">
@@ -3552,14 +3731,14 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="H22" s="21" t="s">
+      <c r="H22" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="28"/>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="5" t="s">
@@ -3567,97 +3746,107 @@
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="41" t="s">
+      <c r="D23" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="H23" s="23" t="s">
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="H23" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="24"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="24"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
     </row>
     <row r="24" spans="1:13">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="H24" s="26" t="s">
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="H24" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="33"/>
     </row>
     <row r="25" spans="1:13">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="H25" s="40" t="s">
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="H25" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I25" s="40"/>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
-      <c r="M25" s="40"/>
+      <c r="I25" s="35"/>
+      <c r="J25" s="35"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="35"/>
+      <c r="M25" s="35"/>
     </row>
     <row r="26" spans="1:13">
-      <c r="A26" s="40" t="s">
+      <c r="A26" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="40"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="40"/>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
-      <c r="M26" s="40"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="35"/>
     </row>
     <row r="27" spans="1:13">
-      <c r="A27" s="40"/>
-      <c r="B27" s="40"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="40"/>
-      <c r="J27" s="40"/>
-      <c r="K27" s="40"/>
-      <c r="L27" s="40"/>
-      <c r="M27" s="40"/>
+      <c r="A27" s="35"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="35"/>
+      <c r="K27" s="35"/>
+      <c r="L27" s="35"/>
+      <c r="M27" s="35"/>
     </row>
     <row r="28" spans="1:13">
-      <c r="H28" s="26" t="s">
+      <c r="H28" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="I28" s="27"/>
-      <c r="J28" s="27"/>
-      <c r="K28" s="27"/>
-      <c r="L28" s="27"/>
-      <c r="M28" s="27"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="33"/>
+      <c r="M28" s="33"/>
     </row>
     <row r="29" spans="1:13" ht="15" customHeight="1">
+      <c r="A29" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
       <c r="H29" s="5" t="s">
         <v>62</v>
       </c>
@@ -3668,46 +3857,90 @@
       <c r="M29" s="1"/>
     </row>
     <row r="30" spans="1:13">
+      <c r="A30" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="H30" s="5" t="s">
         <v>94</v>
       </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
-      <c r="K30" s="41" t="s">
+      <c r="K30" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="L30" s="42"/>
-      <c r="M30" s="42"/>
+      <c r="L30" s="43"/>
+      <c r="M30" s="43"/>
     </row>
     <row r="31" spans="1:13">
-      <c r="H31" s="18" t="s">
+      <c r="A31" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="18"/>
+      <c r="H31" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="I31" s="18"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="26"/>
+      <c r="M31" s="26"/>
     </row>
     <row r="32" spans="1:13">
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-    </row>
-    <row r="33" spans="8:13">
-      <c r="H33" s="26" t="s">
+      <c r="A32" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="26"/>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="18"/>
+      <c r="H33" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="27"/>
-      <c r="L33" s="27"/>
-      <c r="M33" s="27"/>
-    </row>
-    <row r="34" spans="8:13">
+      <c r="I33" s="33"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="33"/>
+      <c r="M33" s="33"/>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
       <c r="H34" s="5" t="s">
         <v>98</v>
       </c>
@@ -3717,39 +3950,75 @@
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
     </row>
-    <row r="35" spans="8:13">
+    <row r="35" spans="1:13">
+      <c r="A35" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
       <c r="H35" s="5" t="s">
         <v>99</v>
       </c>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
-      <c r="K35" s="41" t="s">
+      <c r="K35" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="L35" s="42"/>
-      <c r="M35" s="42"/>
-    </row>
-    <row r="36" spans="8:13" ht="15" customHeight="1">
-      <c r="H36" s="18" t="s">
+      <c r="L35" s="43"/>
+      <c r="M35" s="43"/>
+    </row>
+    <row r="36" spans="1:13" ht="15" customHeight="1">
+      <c r="A36" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="H36" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="I36" s="18"/>
-      <c r="J36" s="18"/>
-      <c r="K36" s="18"/>
-      <c r="L36" s="18"/>
-      <c r="M36" s="18"/>
-    </row>
-    <row r="37" spans="8:13">
-      <c r="H37" s="26" t="s">
+      <c r="I36" s="26"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="26"/>
+      <c r="L36" s="26"/>
+      <c r="M36" s="26"/>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="H37" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="I37" s="27"/>
-      <c r="J37" s="27"/>
-      <c r="K37" s="27"/>
-      <c r="L37" s="27"/>
-      <c r="M37" s="27"/>
-    </row>
-    <row r="38" spans="8:13">
+      <c r="I37" s="33"/>
+      <c r="J37" s="33"/>
+      <c r="K37" s="33"/>
+      <c r="L37" s="33"/>
+      <c r="M37" s="33"/>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
       <c r="H38" s="5" t="s">
         <v>104</v>
       </c>
@@ -3759,46 +4028,126 @@
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
     </row>
-    <row r="39" spans="8:13">
+    <row r="39" spans="1:13">
+      <c r="A39" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
       <c r="H39" s="5" t="s">
         <v>103</v>
       </c>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
-      <c r="K39" s="41" t="s">
+      <c r="K39" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="L39" s="42"/>
-      <c r="M39" s="42"/>
-    </row>
-    <row r="40" spans="8:13" ht="15" customHeight="1">
-      <c r="H40" s="18" t="s">
+      <c r="L39" s="43"/>
+      <c r="M39" s="43"/>
+    </row>
+    <row r="40" spans="1:13" ht="15" customHeight="1">
+      <c r="A40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25"/>
+      <c r="H40" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="I40" s="18"/>
-      <c r="J40" s="18"/>
-      <c r="K40" s="18"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="18"/>
-    </row>
-    <row r="41" spans="8:13">
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="18"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
-    </row>
-    <row r="42" spans="8:13">
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="18"/>
-      <c r="K42" s="18"/>
-      <c r="L42" s="18"/>
-      <c r="M42" s="18"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="26"/>
+      <c r="L40" s="26"/>
+      <c r="M40" s="26"/>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="B41" s="33"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="26"/>
+      <c r="L41" s="26"/>
+      <c r="M41" s="26"/>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="35"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="26"/>
+      <c r="K42" s="26"/>
+      <c r="L42" s="26"/>
+      <c r="M42" s="26"/>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="B44" s="33"/>
+      <c r="C44" s="33"/>
+      <c r="D44" s="33"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="33"/>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45" s="35"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="35"/>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" s="35"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="35"/>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" s="35"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="46">
+  <mergeCells count="58">
     <mergeCell ref="H40:M42"/>
     <mergeCell ref="K35:M35"/>
     <mergeCell ref="H37:M37"/>
@@ -3830,6 +4179,8 @@
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="B18:F18"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A1:C1"/>
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="A24:F24"/>
@@ -3842,11 +4193,22 @@
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B12:F12"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A1:C1"/>
     <mergeCell ref="D9:F9"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A42:F43"/>
+    <mergeCell ref="A45:F47"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="A41:F41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3865,16 +4227,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="34" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -3896,7 +4258,7 @@
       <c r="C3" s="5"/>
       <c r="D3" s="1"/>
       <c r="E3" s="5"/>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="18" t="s">
         <v>59</v>
       </c>
     </row>
@@ -3908,7 +4270,7 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="18" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3918,29 +4280,29 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="18" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="5" t="s">
@@ -3958,65 +4320,65 @@
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1"/>
-      <c r="B13" s="39"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="5" t="s">
@@ -4034,85 +4396,85 @@
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="41" t="s">
+      <c r="D16" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="40"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="40"/>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
+      <c r="A23" s="35"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -4126,12 +4488,12 @@
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B10:F10"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="A7:F7"/>
     <mergeCell ref="D9:F9"/>
-    <mergeCell ref="B10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ivywatch stat blocks, the horror
</commit_message>
<xml_diff>
--- a/adventures/ivywatch/working/monsters.xlsx
+++ b/adventures/ivywatch/working/monsters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gavin\Documents\drawsteel\_products\adventures\ivywatch\working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2375E84E-D82C-4AC8-91F2-5F00D747BA59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054B0DE5-459E-4AE8-AA05-9F1FEA1B18BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1710" yWindow="930" windowWidth="20475" windowHeight="14100" activeTab="2" xr2:uid="{918A4370-6BD2-4549-B40B-132AC3F5AF22}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="157">
   <si>
     <t>[Name]</t>
   </si>
@@ -2114,6 +2114,695 @@
   </si>
   <si>
     <t xml:space="preserve">Might 0    Agility 2    Reason 0    Intuition 1    Presence 0 </t>
+  </si>
+  <si>
+    <t>Level 1 Solo</t>
+  </si>
+  <si>
+    <t>The Horror</t>
+  </si>
+  <si>
+    <t>Undead, Chimera</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Stamina</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (30 * Party Size) + (10 * Victories)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Grafted Arms </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(Action) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>u</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2d10 + 2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>u</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Signature</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Distance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Melee 2</t>
+    </r>
+  </si>
+  <si>
+    <t>4 damage</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5 damage; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A&lt;1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> grabbed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">6 damage; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A&lt;2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> grabbed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Target</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1 creature</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Basilisk Glands </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(Action) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>u</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2d10 + 2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>u</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 5 Malice</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4 poison damage; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>M&lt;0</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> weakened (save ends)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">6 poison damage; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>M&lt;1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> weakened and slowed (save ends)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">9 poison damage; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>M&lt;2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> weakened and slowed (save ends)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Distance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2 Burst</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Effect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The horror can have up to four targets grabbed.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3 Malice </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The horror can vertical push 5 one grabbed target.</t>
+    </r>
+  </si>
+  <si>
+    <t>Arise</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Distance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Ranged 5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Trigger</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The target strikes the horror and gets a tier-1 result.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">6 damage; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A&lt;1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> grabbed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">8 damage; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A&lt;2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> grabbed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10 damage; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A&lt;3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> grabbed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Effect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The horror can have up to four targets grabbed.</t>
+    </r>
+  </si>
+  <si>
+    <t>The first time the horror is reduced to Stamina 0 by damage that isn't fire or holy damage and their body isn't destroyed, they regain 10 Stamina and fall prone.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Kill Them, My Creation! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Triggered Action)</t>
+    </r>
+  </si>
+  <si>
+    <t>Solo Monster</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Solo Turns </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The horror takes up to two turns each round. They can't take turns consecutively.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">End Effect </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>At the end of their turn, the horror can take 5 damage to end one save ends effect affecting them. This damage can't be reduced in any way.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Might +3   Agility -1   Reason +1   Intuition -2   Presence -4 </t>
+  </si>
+  <si>
+    <t>Yslansh's Tactics</t>
+  </si>
+  <si>
+    <t>If the horror would be flanked, Yslansh whispers commands to it and the flankers gain no edge.</t>
+  </si>
+  <si>
+    <t>EV 30</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Size</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2 / </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Stability</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Effect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The horror shifts 5. Any creatures they have grabbed move with the horror, taking 1 damage for each square the horror shifts. If they end this movement adjacent within 2 of the target, roll power.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2304,7 +2993,7 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyBorder="1"/>
@@ -2333,11 +3022,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2348,18 +3034,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="11" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
@@ -2371,31 +3053,60 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="11" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="11" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -2745,16 +3456,16 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="21" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
       <c r="H1" s="8" t="s">
         <v>23</v>
       </c>
@@ -2766,10 +3477,10 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
-      <c r="P1" s="21" t="s">
+      <c r="P1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="21"/>
+      <c r="Q1" s="24"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="2" t="s">
@@ -2895,50 +3606,50 @@
       <c r="Q6" s="1"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
       <c r="H7" s="13" t="s">
         <v>29</v>
       </c>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
-      <c r="L7" s="22" t="s">
+      <c r="L7" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
       <c r="H8" s="14" t="s">
         <v>30</v>
       </c>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
-      <c r="L8" s="24" t="s">
+      <c r="L8" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="5" t="s">
@@ -2994,11 +3705,11 @@
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
       <c r="H11" s="17" t="s">
         <v>33</v>
       </c>
@@ -3007,125 +3718,125 @@
       <c r="L11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="25"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="33"/>
+      <c r="O11" s="33"/>
+      <c r="P11" s="33"/>
+      <c r="Q11" s="33"/>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
       <c r="L12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="25"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="33"/>
+      <c r="P12" s="33"/>
+      <c r="Q12" s="33"/>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
       <c r="L13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="25"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="33"/>
+      <c r="P13" s="33"/>
+      <c r="Q13" s="33"/>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="L14" s="26" t="s">
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="L14" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="26"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="31"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="26"/>
-      <c r="P15" s="26"/>
-      <c r="Q15" s="26"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="31"/>
+      <c r="Q15" s="31"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="26"/>
-      <c r="Q16" s="26"/>
+      <c r="A16" s="31"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="31"/>
+      <c r="Q16" s="31"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="27"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="32"/>
     </row>
     <row r="18" spans="1:17">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="L18" s="24" t="s">
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="L18" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="M18" s="24"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="24"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="23"/>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="5" t="s">
@@ -3151,115 +3862,102 @@
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
       <c r="L20" s="5" t="s">
         <v>11</v>
       </c>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
-      <c r="O20" s="28" t="s">
+      <c r="O20" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="P20" s="29"/>
-      <c r="Q20" s="29"/>
+      <c r="P20" s="35"/>
+      <c r="Q20" s="35"/>
     </row>
     <row r="21" spans="1:17">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="L21" s="30" t="s">
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="L21" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="20"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="27"/>
+      <c r="Q21" s="27"/>
     </row>
     <row r="22" spans="1:17">
-      <c r="A22" s="31"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="31"/>
-      <c r="P22" s="31"/>
-      <c r="Q22" s="31"/>
+      <c r="A22" s="28"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="28"/>
+      <c r="O22" s="28"/>
+      <c r="P22" s="28"/>
+      <c r="Q22" s="28"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="L23" s="32" t="s">
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="L23" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="M23" s="33"/>
-      <c r="N23" s="33"/>
-      <c r="O23" s="33"/>
-      <c r="P23" s="33"/>
-      <c r="Q23" s="33"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="30"/>
+      <c r="P23" s="30"/>
+      <c r="Q23" s="30"/>
     </row>
     <row r="24" spans="1:17">
-      <c r="A24" s="20"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="20"/>
-      <c r="O24" s="20"/>
-      <c r="P24" s="20"/>
-      <c r="Q24" s="20"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="27"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="27"/>
+      <c r="Q24" s="27"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="20"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="L25" s="20"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="20"/>
-      <c r="O25" s="20"/>
-      <c r="P25" s="20"/>
-      <c r="Q25" s="20"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="27"/>
+      <c r="O25" s="27"/>
+      <c r="P25" s="27"/>
+      <c r="Q25" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A21:F22"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="A24:F25"/>
-    <mergeCell ref="A14:F17"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="D20:F20"/>
     <mergeCell ref="L24:Q25"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="L7:Q7"/>
@@ -3272,6 +3970,19 @@
     <mergeCell ref="O20:Q20"/>
     <mergeCell ref="L21:Q22"/>
     <mergeCell ref="L23:Q23"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A24:F25"/>
+    <mergeCell ref="A14:F17"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A21:F22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3292,43 +4003,58 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF82A8B5-C780-4855-A5A0-A052A5BEE04A}">
-  <dimension ref="A1:M47"/>
+  <dimension ref="A1:X45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z39" sqref="Z39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="5" max="5" width="3.85546875" customWidth="1"/>
     <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" customWidth="1"/>
     <col min="12" max="12" width="5.85546875" customWidth="1"/>
     <col min="13" max="13" width="17.85546875" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:24">
+      <c r="A1" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="39" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="H1" s="34" t="s">
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="J1" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="S1" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+    </row>
+    <row r="2" spans="1:24">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -3339,18 +4065,28 @@
       <c r="F2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="S2" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
       <c r="A3" s="5" t="s">
         <v>60</v>
       </c>
@@ -3361,16 +4097,24 @@
       <c r="F3" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="5"/>
       <c r="K3" s="1"/>
       <c r="L3" s="5"/>
-      <c r="M3" s="18"/>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="M3" s="1"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="18"/>
+      <c r="S3" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="T3" s="1"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="18"/>
+    </row>
+    <row r="4" spans="1:24">
       <c r="A4" s="5" t="s">
         <v>38</v>
       </c>
@@ -3381,8 +4125,1126 @@
       <c r="F4" s="18" t="s">
         <v>40</v>
       </c>
+      <c r="J4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
+      <c r="A6" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="J6" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="S6" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="T6" s="22"/>
+      <c r="U6" s="22"/>
+      <c r="V6" s="22"/>
+      <c r="W6" s="22"/>
+      <c r="X6" s="22"/>
+    </row>
+    <row r="7" spans="1:24">
+      <c r="A7" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="J7" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="S7" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29"/>
+      <c r="V7" s="29"/>
+      <c r="W7" s="29"/>
+      <c r="X7" s="29"/>
+    </row>
+    <row r="8" spans="1:24">
+      <c r="A8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="J8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="S8" s="50" t="s">
+        <v>149</v>
+      </c>
+      <c r="T8" s="50"/>
+      <c r="U8" s="50"/>
+      <c r="V8" s="50"/>
+      <c r="W8" s="50"/>
+      <c r="X8" s="50"/>
+    </row>
+    <row r="9" spans="1:24">
+      <c r="A9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="J9" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="N9" s="36"/>
+      <c r="O9" s="36"/>
+      <c r="S9" s="50"/>
+      <c r="T9" s="50"/>
+      <c r="U9" s="50"/>
+      <c r="V9" s="50"/>
+      <c r="W9" s="50"/>
+      <c r="X9" s="50"/>
+    </row>
+    <row r="10" spans="1:24">
+      <c r="A10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="J10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="33"/>
+      <c r="S10" s="50" t="s">
+        <v>150</v>
+      </c>
+      <c r="T10" s="50"/>
+      <c r="U10" s="50"/>
+      <c r="V10" s="50"/>
+      <c r="W10" s="50"/>
+      <c r="X10" s="50"/>
+    </row>
+    <row r="11" spans="1:24">
+      <c r="A11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="J11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="33"/>
+      <c r="O11" s="33"/>
+      <c r="S11" s="50"/>
+      <c r="T11" s="50"/>
+      <c r="U11" s="50"/>
+      <c r="V11" s="50"/>
+      <c r="W11" s="50"/>
+      <c r="X11" s="50"/>
+    </row>
+    <row r="12" spans="1:24">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="J12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K12" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="33"/>
+      <c r="S12" s="50"/>
+      <c r="T12" s="50"/>
+      <c r="U12" s="50"/>
+      <c r="V12" s="50"/>
+      <c r="W12" s="50"/>
+      <c r="X12" s="50"/>
+    </row>
+    <row r="13" spans="1:24">
+      <c r="A13" s="1"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="J13" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="S13" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="T13" s="23"/>
+      <c r="U13" s="23"/>
+      <c r="V13" s="23"/>
+      <c r="W13" s="23"/>
+      <c r="X13" s="23"/>
+    </row>
+    <row r="14" spans="1:24">
+      <c r="A14" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="32"/>
+      <c r="S14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+    </row>
+    <row r="15" spans="1:24">
+      <c r="A15" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="J15" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="S15" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="W15" s="36"/>
+      <c r="X15" s="36"/>
+    </row>
+    <row r="16" spans="1:24">
+      <c r="A16" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="J16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="S16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T16" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="U16" s="33"/>
+      <c r="V16" s="33"/>
+      <c r="W16" s="33"/>
+      <c r="X16" s="33"/>
+    </row>
+    <row r="17" spans="1:24">
+      <c r="A17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="J17" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="N17" s="37"/>
+      <c r="O17" s="37"/>
+      <c r="S17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="T17" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="U17" s="33"/>
+      <c r="V17" s="33"/>
+      <c r="W17" s="33"/>
+      <c r="X17" s="33"/>
+    </row>
+    <row r="18" spans="1:24">
+      <c r="A18" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="J18" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="27"/>
+      <c r="O18" s="27"/>
+      <c r="S18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T18" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="U18" s="33"/>
+      <c r="V18" s="33"/>
+      <c r="W18" s="33"/>
+      <c r="X18" s="33"/>
+    </row>
+    <row r="19" spans="1:24">
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="J19" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="S19" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="T19" s="31"/>
+      <c r="U19" s="31"/>
+      <c r="V19" s="31"/>
+      <c r="W19" s="31"/>
+      <c r="X19" s="31"/>
+    </row>
+    <row r="20" spans="1:24">
+      <c r="A20" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="J20" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="S20" s="32"/>
+      <c r="T20" s="32"/>
+      <c r="U20" s="32"/>
+      <c r="V20" s="32"/>
+      <c r="W20" s="32"/>
+      <c r="X20" s="32"/>
+    </row>
+    <row r="21" spans="1:24">
+      <c r="A21" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="J21" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="N21" s="37"/>
+      <c r="O21" s="37"/>
+      <c r="S21" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="T21" s="23"/>
+      <c r="U21" s="23"/>
+      <c r="V21" s="23"/>
+      <c r="W21" s="23"/>
+      <c r="X21" s="23"/>
+    </row>
+    <row r="22" spans="1:24">
+      <c r="A22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="J22" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="34"/>
+      <c r="S22" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+    </row>
+    <row r="23" spans="1:24">
+      <c r="A23" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="J23" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="27"/>
+      <c r="O23" s="27"/>
+      <c r="S23" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="W23" s="36"/>
+      <c r="X23" s="36"/>
+    </row>
+    <row r="24" spans="1:24">
+      <c r="A24" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="J24" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="30"/>
+      <c r="S24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T24" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="U24" s="33"/>
+      <c r="V24" s="33"/>
+      <c r="W24" s="33"/>
+      <c r="X24" s="33"/>
+    </row>
+    <row r="25" spans="1:24">
+      <c r="A25" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="J25" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="K25" s="38"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="38"/>
+      <c r="S25" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="T25" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="U25" s="33"/>
+      <c r="V25" s="33"/>
+      <c r="W25" s="33"/>
+      <c r="X25" s="33"/>
+    </row>
+    <row r="26" spans="1:24">
+      <c r="A26" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="38"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="38"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="38"/>
+      <c r="S26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T26" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="U26" s="33"/>
+      <c r="V26" s="33"/>
+      <c r="W26" s="33"/>
+      <c r="X26" s="33"/>
+    </row>
+    <row r="27" spans="1:24">
+      <c r="A27" s="38"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="38"/>
+      <c r="L27" s="38"/>
+      <c r="M27" s="38"/>
+      <c r="N27" s="38"/>
+      <c r="O27" s="38"/>
+      <c r="S27" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="T27" s="30"/>
+      <c r="U27" s="30"/>
+      <c r="V27" s="30"/>
+      <c r="W27" s="30"/>
+      <c r="X27" s="30"/>
+    </row>
+    <row r="28" spans="1:24" ht="15" customHeight="1">
+      <c r="J28" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="30"/>
+      <c r="N28" s="30"/>
+      <c r="O28" s="30"/>
+      <c r="S28" s="51" t="s">
+        <v>153</v>
+      </c>
+      <c r="T28" s="51"/>
+      <c r="U28" s="51"/>
+      <c r="V28" s="51"/>
+      <c r="W28" s="51"/>
+      <c r="X28" s="51"/>
+    </row>
+    <row r="29" spans="1:24" ht="15" customHeight="1">
+      <c r="J29" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="S29" s="47"/>
+      <c r="T29" s="47"/>
+      <c r="U29" s="47"/>
+      <c r="V29" s="47"/>
+      <c r="W29" s="47"/>
+      <c r="X29" s="47"/>
+    </row>
+    <row r="30" spans="1:24">
+      <c r="J30" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="N30" s="37"/>
+      <c r="O30" s="37"/>
+      <c r="S30" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="T30" s="23"/>
+      <c r="U30" s="23"/>
+      <c r="V30" s="23"/>
+      <c r="W30" s="23"/>
+      <c r="X30" s="23"/>
+    </row>
+    <row r="31" spans="1:24">
+      <c r="J31" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="K31" s="31"/>
+      <c r="L31" s="31"/>
+      <c r="M31" s="31"/>
+      <c r="N31" s="31"/>
+      <c r="O31" s="31"/>
+      <c r="S31" s="45" t="s">
+        <v>146</v>
+      </c>
+      <c r="T31" s="45"/>
+      <c r="U31" s="45"/>
+      <c r="V31" s="45"/>
+      <c r="W31" s="45"/>
+      <c r="X31" s="45"/>
+    </row>
+    <row r="32" spans="1:24">
+      <c r="J32" s="31"/>
+      <c r="K32" s="31"/>
+      <c r="L32" s="31"/>
+      <c r="M32" s="31"/>
+      <c r="N32" s="31"/>
+      <c r="O32" s="31"/>
+      <c r="S32" s="45"/>
+      <c r="T32" s="45"/>
+      <c r="U32" s="45"/>
+      <c r="V32" s="45"/>
+      <c r="W32" s="45"/>
+      <c r="X32" s="45"/>
+    </row>
+    <row r="33" spans="10:24">
+      <c r="J33" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="K33" s="30"/>
+      <c r="L33" s="30"/>
+      <c r="M33" s="30"/>
+      <c r="N33" s="30"/>
+      <c r="O33" s="30"/>
+      <c r="S33" s="46"/>
+      <c r="T33" s="46"/>
+      <c r="U33" s="46"/>
+      <c r="V33" s="46"/>
+      <c r="W33" s="46"/>
+      <c r="X33" s="46"/>
+    </row>
+    <row r="34" spans="10:24">
+      <c r="J34" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="S34" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="T34" s="23"/>
+      <c r="U34" s="23"/>
+      <c r="V34" s="23"/>
+      <c r="W34" s="23"/>
+      <c r="X34" s="23"/>
+    </row>
+    <row r="35" spans="10:24">
+      <c r="J35" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="N35" s="37"/>
+      <c r="O35" s="37"/>
+      <c r="S35" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="1"/>
+      <c r="X35" s="1"/>
+    </row>
+    <row r="36" spans="10:24" ht="15" customHeight="1">
+      <c r="J36" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="K36" s="31"/>
+      <c r="L36" s="31"/>
+      <c r="M36" s="31"/>
+      <c r="N36" s="31"/>
+      <c r="O36" s="31"/>
+      <c r="S36" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="W36" s="37"/>
+      <c r="X36" s="37"/>
+    </row>
+    <row r="37" spans="10:24">
+      <c r="J37" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="K37" s="30"/>
+      <c r="L37" s="30"/>
+      <c r="M37" s="30"/>
+      <c r="N37" s="30"/>
+      <c r="O37" s="30"/>
+      <c r="S37" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="T37" s="34"/>
+      <c r="U37" s="34"/>
+      <c r="V37" s="34"/>
+      <c r="W37" s="34"/>
+      <c r="X37" s="34"/>
+    </row>
+    <row r="38" spans="10:24">
+      <c r="J38" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="S38" s="45" t="s">
+        <v>156</v>
+      </c>
+      <c r="T38" s="45"/>
+      <c r="U38" s="45"/>
+      <c r="V38" s="45"/>
+      <c r="W38" s="45"/>
+      <c r="X38" s="45"/>
+    </row>
+    <row r="39" spans="10:24">
+      <c r="J39" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="N39" s="37"/>
+      <c r="O39" s="37"/>
+      <c r="S39" s="45"/>
+      <c r="T39" s="45"/>
+      <c r="U39" s="45"/>
+      <c r="V39" s="45"/>
+      <c r="W39" s="45"/>
+      <c r="X39" s="45"/>
+    </row>
+    <row r="40" spans="10:24" ht="15" customHeight="1">
+      <c r="J40" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="K40" s="31"/>
+      <c r="L40" s="31"/>
+      <c r="M40" s="31"/>
+      <c r="N40" s="31"/>
+      <c r="O40" s="31"/>
+      <c r="S40" s="45"/>
+      <c r="T40" s="45"/>
+      <c r="U40" s="45"/>
+      <c r="V40" s="45"/>
+      <c r="W40" s="45"/>
+      <c r="X40" s="45"/>
+    </row>
+    <row r="41" spans="10:24">
+      <c r="J41" s="31"/>
+      <c r="K41" s="31"/>
+      <c r="L41" s="31"/>
+      <c r="M41" s="31"/>
+      <c r="N41" s="31"/>
+      <c r="O41" s="31"/>
+      <c r="S41" s="45"/>
+      <c r="T41" s="45"/>
+      <c r="U41" s="45"/>
+      <c r="V41" s="45"/>
+      <c r="W41" s="45"/>
+      <c r="X41" s="45"/>
+    </row>
+    <row r="42" spans="10:24">
+      <c r="J42" s="31"/>
+      <c r="K42" s="31"/>
+      <c r="L42" s="31"/>
+      <c r="M42" s="31"/>
+      <c r="N42" s="31"/>
+      <c r="O42" s="31"/>
+      <c r="S42" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T42" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="U42" s="33"/>
+      <c r="V42" s="33"/>
+      <c r="W42" s="33"/>
+      <c r="X42" s="33"/>
+    </row>
+    <row r="43" spans="10:24" ht="15" customHeight="1">
+      <c r="S43" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="T43" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="U43" s="33"/>
+      <c r="V43" s="33"/>
+      <c r="W43" s="33"/>
+      <c r="X43" s="33"/>
+    </row>
+    <row r="44" spans="10:24">
+      <c r="O44" s="49"/>
+      <c r="P44" s="49"/>
+      <c r="Q44" s="49"/>
+      <c r="R44" s="49"/>
+      <c r="S44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T44" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="U44" s="7"/>
+      <c r="V44" s="7"/>
+      <c r="W44" s="7"/>
+      <c r="X44" s="7"/>
+    </row>
+    <row r="45" spans="10:24">
+      <c r="S45" s="48" t="s">
+        <v>145</v>
+      </c>
+      <c r="T45" s="48"/>
+      <c r="U45" s="48"/>
+      <c r="V45" s="48"/>
+      <c r="W45" s="48"/>
+      <c r="X45" s="48"/>
+    </row>
+  </sheetData>
+  <mergeCells count="74">
+    <mergeCell ref="S13:X13"/>
+    <mergeCell ref="V15:X15"/>
+    <mergeCell ref="T16:X16"/>
+    <mergeCell ref="T17:X17"/>
+    <mergeCell ref="T18:X18"/>
+    <mergeCell ref="S19:X20"/>
+    <mergeCell ref="S31:X33"/>
+    <mergeCell ref="T42:X42"/>
+    <mergeCell ref="T43:X43"/>
+    <mergeCell ref="S38:X41"/>
+    <mergeCell ref="S28:X29"/>
+    <mergeCell ref="S45:X45"/>
+    <mergeCell ref="S34:X34"/>
+    <mergeCell ref="V36:X36"/>
+    <mergeCell ref="S37:X37"/>
+    <mergeCell ref="S27:X27"/>
+    <mergeCell ref="T24:X24"/>
+    <mergeCell ref="T25:X25"/>
+    <mergeCell ref="T26:X26"/>
+    <mergeCell ref="S30:X30"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="S6:X6"/>
+    <mergeCell ref="S21:X21"/>
+    <mergeCell ref="V23:X23"/>
+    <mergeCell ref="S7:X7"/>
+    <mergeCell ref="S8:X9"/>
+    <mergeCell ref="S10:X12"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A26:F27"/>
+    <mergeCell ref="J13:O14"/>
+    <mergeCell ref="J19:O19"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="J6:O6"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="K10:O10"/>
+    <mergeCell ref="K11:O11"/>
+    <mergeCell ref="K12:O12"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="M30:O30"/>
+    <mergeCell ref="J31:O32"/>
+    <mergeCell ref="J33:O33"/>
+    <mergeCell ref="J25:O27"/>
+    <mergeCell ref="J15:O15"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="J18:O18"/>
+    <mergeCell ref="J22:O22"/>
+    <mergeCell ref="J28:O28"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="J23:O23"/>
+    <mergeCell ref="J24:O24"/>
+    <mergeCell ref="J40:O42"/>
+    <mergeCell ref="M35:O35"/>
+    <mergeCell ref="J37:O37"/>
+    <mergeCell ref="M39:O39"/>
+    <mergeCell ref="J36:O36"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02DFD280-CB3F-4A45-8F62-9CF1F8B27A7E}">
+  <dimension ref="A1:M23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="5" width="4.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="H1" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="18"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="18" t="s">
+        <v>40</v>
+      </c>
       <c r="H4" s="5" t="s">
-        <v>73</v>
+        <v>111</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -3401,50 +5263,50 @@
       <c r="F5" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="1"/>
+      <c r="H5" s="5" t="s">
+        <v>121</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="18" t="s">
-        <v>81</v>
-      </c>
+      <c r="M5" s="18"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="H6" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="H6" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="H7" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="H7" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="5" t="s">
@@ -3456,7 +5318,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="H8" s="5" t="s">
-        <v>43</v>
+        <v>115</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -3470,87 +5332,87 @@
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="37" t="s">
+      <c r="D9" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="H9" s="5" t="s">
-        <v>87</v>
+        <v>44</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37"/>
+      <c r="K9" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="L9" s="36"/>
+      <c r="M9" s="36"/>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
       <c r="H10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
+      <c r="I10" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
       <c r="H11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
+      <c r="I11" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
       <c r="H12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
+      <c r="I12" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="1"/>
@@ -3559,30 +5421,32 @@
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
-      <c r="H13" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
+      <c r="H13" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="27"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="H14" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="5" t="s">
@@ -3593,14 +5457,12 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="H15" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="5" t="s">
@@ -3608,876 +5470,134 @@
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="37" t="s">
+      <c r="D16" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="H16" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="H16" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="H17" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="L17" s="43"/>
-      <c r="M17" s="43"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="H17" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="H18" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="H19" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="H20" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
     </row>
     <row r="21" spans="1:13">
-      <c r="A21" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="H21" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="L21" s="43"/>
-      <c r="M21" s="43"/>
+      <c r="A21" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
     </row>
     <row r="22" spans="1:13">
-      <c r="A22" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="H22" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
+      <c r="A22" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
     </row>
     <row r="23" spans="1:13">
-      <c r="A23" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
-      <c r="H23" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="A24" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="H24" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-    </row>
-    <row r="25" spans="1:13">
-      <c r="A25" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="H25" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="I25" s="35"/>
-      <c r="J25" s="35"/>
-      <c r="K25" s="35"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="35"/>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="A26" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" s="35"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
-      <c r="J26" s="35"/>
-      <c r="K26" s="35"/>
-      <c r="L26" s="35"/>
-      <c r="M26" s="35"/>
-    </row>
-    <row r="27" spans="1:13">
-      <c r="A27" s="35"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="35"/>
-      <c r="K27" s="35"/>
-      <c r="L27" s="35"/>
-      <c r="M27" s="35"/>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="H28" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="I28" s="33"/>
-      <c r="J28" s="33"/>
-      <c r="K28" s="33"/>
-      <c r="L28" s="33"/>
-      <c r="M28" s="33"/>
-    </row>
-    <row r="29" spans="1:13" ht="15" customHeight="1">
-      <c r="A29" s="38" t="s">
-        <v>107</v>
-      </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="H29" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="37" t="s">
-        <v>95</v>
-      </c>
-      <c r="L30" s="43"/>
-      <c r="M30" s="43"/>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="18"/>
-      <c r="H31" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26"/>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="26"/>
-      <c r="L32" s="26"/>
-      <c r="M32" s="26"/>
-    </row>
-    <row r="33" spans="1:13">
-      <c r="A33" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="18"/>
-      <c r="H33" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="I33" s="33"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="33"/>
-      <c r="L33" s="33"/>
-      <c r="M33" s="33"/>
-    </row>
-    <row r="34" spans="1:13">
-      <c r="A34" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="H34" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-    </row>
-    <row r="35" spans="1:13">
-      <c r="A35" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="H35" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="37" t="s">
-        <v>100</v>
-      </c>
-      <c r="L35" s="43"/>
-      <c r="M35" s="43"/>
-    </row>
-    <row r="36" spans="1:13" ht="15" customHeight="1">
-      <c r="A36" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="H36" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="I36" s="26"/>
-      <c r="J36" s="26"/>
-      <c r="K36" s="26"/>
-      <c r="L36" s="26"/>
-      <c r="M36" s="26"/>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
-      <c r="H37" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="I37" s="33"/>
-      <c r="J37" s="33"/>
-      <c r="K37" s="33"/>
-      <c r="L37" s="33"/>
-      <c r="M37" s="33"/>
-    </row>
-    <row r="38" spans="1:13">
-      <c r="A38" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B38" s="36" t="s">
-        <v>116</v>
-      </c>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="H38" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-    </row>
-    <row r="39" spans="1:13">
-      <c r="A39" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B39" s="36" t="s">
-        <v>117</v>
-      </c>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="H39" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="37" t="s">
-        <v>105</v>
-      </c>
-      <c r="L39" s="43"/>
-      <c r="M39" s="43"/>
-    </row>
-    <row r="40" spans="1:13" ht="15" customHeight="1">
-      <c r="A40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B40" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="H40" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="I40" s="26"/>
-      <c r="J40" s="26"/>
-      <c r="K40" s="26"/>
-      <c r="L40" s="26"/>
-      <c r="M40" s="26"/>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="B41" s="33"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="33"/>
-      <c r="H41" s="26"/>
-      <c r="I41" s="26"/>
-      <c r="J41" s="26"/>
-      <c r="K41" s="26"/>
-      <c r="L41" s="26"/>
-      <c r="M41" s="26"/>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="A42" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="B42" s="35"/>
-      <c r="C42" s="35"/>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="35"/>
-      <c r="H42" s="26"/>
-      <c r="I42" s="26"/>
-      <c r="J42" s="26"/>
-      <c r="K42" s="26"/>
-      <c r="L42" s="26"/>
-      <c r="M42" s="26"/>
-    </row>
-    <row r="43" spans="1:13">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
-      <c r="C43" s="35"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="35"/>
-    </row>
-    <row r="44" spans="1:13">
-      <c r="A44" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="B44" s="33"/>
-      <c r="C44" s="33"/>
-      <c r="D44" s="33"/>
-      <c r="E44" s="33"/>
-      <c r="F44" s="33"/>
-    </row>
-    <row r="45" spans="1:13">
-      <c r="A45" s="35" t="s">
-        <v>120</v>
-      </c>
-      <c r="B45" s="35"/>
-      <c r="C45" s="35"/>
-      <c r="D45" s="35"/>
-      <c r="E45" s="35"/>
-      <c r="F45" s="35"/>
-    </row>
-    <row r="46" spans="1:13">
-      <c r="A46" s="35"/>
-      <c r="B46" s="35"/>
-      <c r="C46" s="35"/>
-      <c r="D46" s="35"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="35"/>
-    </row>
-    <row r="47" spans="1:13">
-      <c r="A47" s="35"/>
-      <c r="B47" s="35"/>
-      <c r="C47" s="35"/>
-      <c r="D47" s="35"/>
-      <c r="E47" s="35"/>
-      <c r="F47" s="35"/>
+      <c r="A23" s="38"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="58">
-    <mergeCell ref="H40:M42"/>
-    <mergeCell ref="K35:M35"/>
-    <mergeCell ref="H37:M37"/>
-    <mergeCell ref="K39:M39"/>
-    <mergeCell ref="H36:M36"/>
-    <mergeCell ref="K30:M30"/>
-    <mergeCell ref="H31:M32"/>
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="H25:M27"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="H18:M18"/>
-    <mergeCell ref="H22:M22"/>
-    <mergeCell ref="H28:M28"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="H23:M23"/>
-    <mergeCell ref="H24:M24"/>
-    <mergeCell ref="H13:M14"/>
-    <mergeCell ref="H19:M19"/>
-    <mergeCell ref="B19:F19"/>
+  <mergeCells count="28">
+    <mergeCell ref="H7:M7"/>
+    <mergeCell ref="K9:M9"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="H6:M6"/>
-    <mergeCell ref="H7:M7"/>
-    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="H14:M15"/>
+    <mergeCell ref="H17:M19"/>
     <mergeCell ref="I10:M10"/>
     <mergeCell ref="I11:M11"/>
     <mergeCell ref="I12:M12"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="A26:F27"/>
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="A14:F14"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="A7:F7"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
     <mergeCell ref="D9:F9"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A42:F43"/>
-    <mergeCell ref="A45:F47"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="A41:F41"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02DFD280-CB3F-4A45-8F62-9CF1F8B27A7E}">
-  <dimension ref="A1:F23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="5" max="5" width="4.140625" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="1"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="B22" s="35"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="35"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-    </row>
-  </sheetData>
-  <mergeCells count="16">
     <mergeCell ref="A22:F23"/>
     <mergeCell ref="B19:F19"/>
     <mergeCell ref="A20:F20"/>
@@ -4488,12 +5608,6 @@
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="D9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ivywatch post playtest fixes
</commit_message>
<xml_diff>
--- a/adventures/ivywatch/working/monsters.xlsx
+++ b/adventures/ivywatch/working/monsters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gavin\Documents\drawsteel\_products\adventures\ivywatch\working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8BB19D-BBB9-4CCE-8A08-3BA5C4382A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F88BDF3-2BA9-471B-BD82-23D6BC284318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="1080" windowWidth="20475" windowHeight="14100" activeTab="2" xr2:uid="{918A4370-6BD2-4549-B40B-132AC3F5AF22}"/>
+    <workbookView xWindow="1050" yWindow="735" windowWidth="20475" windowHeight="14100" activeTab="3" xr2:uid="{918A4370-6BD2-4549-B40B-132AC3F5AF22}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -3024,21 +3024,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Effect </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Bleddyn and her mentor, if they're within 5 squares from Bleddyn, can shift 2 before the ability is used.</t>
-    </r>
-  </si>
-  <si>
     <t>Unwavering in the Storm</t>
   </si>
   <si>
@@ -6207,6 +6192,21 @@
         <scheme val="minor"/>
       </rPr>
       <t>The horror can vertical push 5 two creatures among either the targets or creatures it has grabbed.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Effect </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bleddyn and their mentor, if they're within 5 squares from Bleddyn, can shift 2 before the ability is used.</t>
     </r>
   </si>
 </sst>
@@ -6502,6 +6502,12 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -6525,12 +6531,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -7472,7 +7472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF82A8B5-C780-4855-A5A0-A052A5BEE04A}">
   <dimension ref="A1:CR71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="L7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AA25" sqref="AA25"/>
     </sheetView>
   </sheetViews>
@@ -7527,85 +7527,85 @@
       </c>
       <c r="W1" s="30"/>
       <c r="X1" s="30"/>
-      <c r="AB1" s="47" t="s">
+      <c r="AB1" s="49" t="s">
+        <v>181</v>
+      </c>
+      <c r="AC1" s="50"/>
+      <c r="AD1" s="50"/>
+      <c r="AE1" s="51" t="s">
         <v>182</v>
       </c>
-      <c r="AC1" s="48"/>
-      <c r="AD1" s="48"/>
-      <c r="AE1" s="49" t="s">
-        <v>183</v>
-      </c>
-      <c r="AF1" s="50"/>
-      <c r="AG1" s="50"/>
+      <c r="AF1" s="52"/>
+      <c r="AG1" s="52"/>
       <c r="AK1" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AL1" s="25"/>
       <c r="AM1" s="25"/>
       <c r="AN1" s="25"/>
       <c r="AO1" s="25"/>
       <c r="AP1" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AT1" s="23" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AU1" s="17"/>
       <c r="AV1" s="17"/>
       <c r="AW1" s="17"/>
       <c r="AX1" s="17"/>
       <c r="AY1" s="27" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="BC1" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="BD1" s="3"/>
       <c r="BE1" s="3"/>
       <c r="BF1" s="22"/>
       <c r="BG1" s="22"/>
       <c r="BH1" s="22" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="BL1" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="BM1" s="3"/>
       <c r="BN1" s="3"/>
       <c r="BO1" s="22"/>
       <c r="BP1" s="22"/>
       <c r="BQ1" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="BU1" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="BV1" s="3"/>
       <c r="BW1" s="3"/>
       <c r="BX1" s="22"/>
       <c r="BY1" s="22"/>
       <c r="BZ1" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="CD1" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="CE1" s="3"/>
       <c r="CF1" s="3"/>
       <c r="CG1" s="22"/>
       <c r="CH1" s="22"/>
       <c r="CI1" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="CM1" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="CN1" s="17"/>
       <c r="CO1" s="17"/>
       <c r="CP1" s="17"/>
       <c r="CQ1" s="17"/>
       <c r="CR1" s="27" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:96">
@@ -7640,57 +7640,57 @@
         <v>148</v>
       </c>
       <c r="AB2" s="21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
       <c r="AF2" s="4"/>
       <c r="AG2" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AK2" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AL2" s="2"/>
       <c r="AM2" s="2"/>
       <c r="AN2" s="2"/>
       <c r="AO2" s="4"/>
       <c r="AP2" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AT2" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AU2" s="2"/>
       <c r="AV2" s="2"/>
       <c r="AW2" s="2"/>
       <c r="AX2" s="4"/>
       <c r="AY2" s="24" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="BC2" s="21" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="BD2" s="2"/>
       <c r="BE2" s="2"/>
       <c r="BF2" s="2"/>
       <c r="BG2" s="2"/>
       <c r="BH2" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="BL2" s="21" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="BM2" s="2"/>
       <c r="BN2" s="2"/>
       <c r="BO2" s="2"/>
       <c r="BP2" s="2"/>
       <c r="BQ2" s="24" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="BU2" s="44" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="BV2" s="44"/>
       <c r="BW2" s="44"/>
@@ -7698,7 +7698,7 @@
       <c r="BY2" s="44"/>
       <c r="BZ2" s="44"/>
       <c r="CD2" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="CE2" s="2"/>
       <c r="CF2" s="2"/>
@@ -7708,14 +7708,14 @@
         <v>148</v>
       </c>
       <c r="CM2" s="21" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="CN2" s="2"/>
       <c r="CO2" s="2"/>
       <c r="CP2" s="2"/>
       <c r="CQ2" s="4"/>
       <c r="CR2" s="24" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:96">
@@ -7746,37 +7746,37 @@
       <c r="W3" s="5"/>
       <c r="X3" s="18"/>
       <c r="AB3" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AC3" s="1"/>
       <c r="AD3" s="5"/>
       <c r="AE3" s="1"/>
       <c r="AF3" s="5"/>
       <c r="AG3" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AK3" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AL3" s="1"/>
       <c r="AM3" s="5"/>
       <c r="AN3" s="1"/>
       <c r="AO3" s="5"/>
       <c r="AP3" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AT3" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AU3" s="1"/>
       <c r="AV3" s="5"/>
       <c r="AW3" s="1"/>
       <c r="AX3" s="5"/>
       <c r="AY3" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="BC3" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="BD3" s="1"/>
       <c r="BE3" s="5"/>
@@ -7786,21 +7786,21 @@
         <v>40</v>
       </c>
       <c r="BL3" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="BM3" s="1"/>
       <c r="BN3" s="5"/>
       <c r="BO3" s="1"/>
       <c r="BP3" s="5"/>
       <c r="BQ3" s="18" t="s">
-        <v>320</v>
-      </c>
-      <c r="BU3" s="54"/>
-      <c r="BV3" s="54"/>
-      <c r="BW3" s="54"/>
-      <c r="BX3" s="54"/>
-      <c r="BY3" s="54"/>
-      <c r="BZ3" s="54"/>
+        <v>319</v>
+      </c>
+      <c r="BU3" s="56"/>
+      <c r="BV3" s="56"/>
+      <c r="BW3" s="56"/>
+      <c r="BX3" s="56"/>
+      <c r="BY3" s="56"/>
+      <c r="BZ3" s="56"/>
       <c r="CD3" s="5" t="s">
         <v>122</v>
       </c>
@@ -7810,7 +7810,7 @@
       <c r="CH3" s="5"/>
       <c r="CI3" s="18"/>
       <c r="CM3" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="CN3" s="1"/>
       <c r="CO3" s="5"/>
@@ -7859,10 +7859,10 @@
       <c r="AE4" s="1"/>
       <c r="AF4" s="5"/>
       <c r="AG4" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AK4" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AL4" s="1"/>
       <c r="AM4" s="1"/>
@@ -7872,7 +7872,7 @@
         <v>40</v>
       </c>
       <c r="AT4" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
@@ -7902,7 +7902,7 @@
         <v>81</v>
       </c>
       <c r="BU4" s="33" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="BV4" s="33"/>
       <c r="BW4" s="33"/>
@@ -7920,7 +7920,7 @@
         <v>149</v>
       </c>
       <c r="CM4" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="CN4" s="1"/>
       <c r="CO4" s="1"/>
@@ -7956,7 +7956,7 @@
         <v>81</v>
       </c>
       <c r="AB5" s="37" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AC5" s="37"/>
       <c r="AD5" s="37"/>
@@ -7966,14 +7966,14 @@
         <v>39</v>
       </c>
       <c r="AK5" s="37" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AL5" s="37"/>
       <c r="AM5" s="37"/>
       <c r="AN5" s="37"/>
       <c r="AO5" s="1"/>
       <c r="AP5" s="18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AT5" s="37"/>
       <c r="AU5" s="37"/>
@@ -7984,7 +7984,7 @@
         <v>118</v>
       </c>
       <c r="BC5" s="31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="BD5" s="32"/>
       <c r="BE5" s="32"/>
@@ -7992,7 +7992,7 @@
       <c r="BG5" s="32"/>
       <c r="BH5" s="32"/>
       <c r="BL5" s="31" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="BM5" s="32"/>
       <c r="BN5" s="32"/>
@@ -8000,7 +8000,7 @@
       <c r="BP5" s="32"/>
       <c r="BQ5" s="32"/>
       <c r="BU5" s="44" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="BV5" s="44"/>
       <c r="BW5" s="44"/>
@@ -8016,7 +8016,7 @@
         <v>81</v>
       </c>
       <c r="CM5" s="31" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="CN5" s="32"/>
       <c r="CO5" s="32"/>
@@ -8050,7 +8050,7 @@
       <c r="W6" s="32"/>
       <c r="X6" s="32"/>
       <c r="AB6" s="31" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AC6" s="32"/>
       <c r="AD6" s="32"/>
@@ -8058,7 +8058,7 @@
       <c r="AF6" s="32"/>
       <c r="AG6" s="32"/>
       <c r="AK6" s="31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AL6" s="32"/>
       <c r="AM6" s="32"/>
@@ -8066,7 +8066,7 @@
       <c r="AO6" s="32"/>
       <c r="AP6" s="32"/>
       <c r="AT6" s="31" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AU6" s="32"/>
       <c r="AV6" s="32"/>
@@ -8074,7 +8074,7 @@
       <c r="AX6" s="32"/>
       <c r="AY6" s="32"/>
       <c r="BC6" s="33" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BD6" s="33"/>
       <c r="BE6" s="33"/>
@@ -8089,12 +8089,12 @@
       <c r="BO6" s="41"/>
       <c r="BP6" s="41"/>
       <c r="BQ6" s="41"/>
-      <c r="BU6" s="54"/>
-      <c r="BV6" s="54"/>
-      <c r="BW6" s="54"/>
-      <c r="BX6" s="54"/>
-      <c r="BY6" s="54"/>
-      <c r="BZ6" s="54"/>
+      <c r="BU6" s="56"/>
+      <c r="BV6" s="56"/>
+      <c r="BW6" s="56"/>
+      <c r="BX6" s="56"/>
+      <c r="BY6" s="56"/>
+      <c r="BZ6" s="56"/>
       <c r="CD6" s="31" t="s">
         <v>145</v>
       </c>
@@ -8104,7 +8104,7 @@
       <c r="CH6" s="32"/>
       <c r="CI6" s="32"/>
       <c r="CM6" s="33" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="CN6" s="33"/>
       <c r="CO6" s="33"/>
@@ -8138,7 +8138,7 @@
       <c r="W7" s="41"/>
       <c r="X7" s="41"/>
       <c r="AB7" s="33" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AC7" s="33"/>
       <c r="AD7" s="33"/>
@@ -8146,7 +8146,7 @@
       <c r="AF7" s="33"/>
       <c r="AG7" s="33"/>
       <c r="AK7" s="33" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AL7" s="33"/>
       <c r="AM7" s="33"/>
@@ -8154,7 +8154,7 @@
       <c r="AO7" s="33"/>
       <c r="AP7" s="33"/>
       <c r="AT7" s="33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AU7" s="33"/>
       <c r="AV7" s="33"/>
@@ -8162,7 +8162,7 @@
       <c r="AX7" s="33"/>
       <c r="AY7" s="33"/>
       <c r="BC7" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="BD7" s="1"/>
       <c r="BE7" s="1"/>
@@ -8178,7 +8178,7 @@
       <c r="BP7" s="45"/>
       <c r="BQ7" s="45"/>
       <c r="BU7" s="33" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="BV7" s="33"/>
       <c r="BW7" s="33"/>
@@ -8186,7 +8186,7 @@
       <c r="BY7" s="33"/>
       <c r="BZ7" s="33"/>
       <c r="CD7" s="33" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="CE7" s="33"/>
       <c r="CF7" s="33"/>
@@ -8228,7 +8228,7 @@
       <c r="W8" s="45"/>
       <c r="X8" s="45"/>
       <c r="AB8" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
@@ -8244,7 +8244,7 @@
       <c r="AO8" s="1"/>
       <c r="AP8" s="1"/>
       <c r="AT8" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AU8" s="1"/>
       <c r="AV8" s="1"/>
@@ -8259,7 +8259,7 @@
       <c r="BF8" s="18"/>
       <c r="BG8" s="18"/>
       <c r="BH8" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="BL8" s="45"/>
       <c r="BM8" s="45"/>
@@ -8268,7 +8268,7 @@
       <c r="BP8" s="45"/>
       <c r="BQ8" s="45"/>
       <c r="BU8" s="44" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="BV8" s="44"/>
       <c r="BW8" s="44"/>
@@ -8284,14 +8284,14 @@
       <c r="CH8" s="1"/>
       <c r="CI8" s="1"/>
       <c r="CM8" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="CN8" s="1"/>
       <c r="CO8" s="1"/>
       <c r="CP8" s="18"/>
       <c r="CQ8" s="18"/>
       <c r="CR8" s="18" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:96">
@@ -8300,21 +8300,21 @@
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="55" t="s">
+      <c r="D9" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
       <c r="J9" s="5" t="s">
         <v>87</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="55" t="s">
+      <c r="M9" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="N9" s="55"/>
-      <c r="O9" s="55"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="47"/>
       <c r="S9" s="45"/>
       <c r="T9" s="45"/>
       <c r="U9" s="45"/>
@@ -8322,14 +8322,14 @@
       <c r="W9" s="45"/>
       <c r="X9" s="45"/>
       <c r="AB9" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
       <c r="AE9" s="18"/>
       <c r="AF9" s="18"/>
       <c r="AG9" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AK9" s="5" t="s">
         <v>123</v>
@@ -8339,7 +8339,7 @@
       <c r="AN9" s="18"/>
       <c r="AO9" s="18"/>
       <c r="AP9" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AT9" s="5" t="s">
         <v>103</v>
@@ -8349,13 +8349,13 @@
       <c r="AW9" s="18"/>
       <c r="AX9" s="18"/>
       <c r="AY9" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="BC9" s="6" t="s">
         <v>8</v>
       </c>
       <c r="BD9" s="46" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="BE9" s="34"/>
       <c r="BF9" s="34"/>
@@ -8369,27 +8369,27 @@
       <c r="BO9" s="45"/>
       <c r="BP9" s="45"/>
       <c r="BQ9" s="45"/>
-      <c r="BU9" s="54"/>
-      <c r="BV9" s="54"/>
-      <c r="BW9" s="54"/>
-      <c r="BX9" s="54"/>
-      <c r="BY9" s="54"/>
-      <c r="BZ9" s="54"/>
+      <c r="BU9" s="56"/>
+      <c r="BV9" s="56"/>
+      <c r="BW9" s="56"/>
+      <c r="BX9" s="56"/>
+      <c r="BY9" s="56"/>
+      <c r="BZ9" s="56"/>
       <c r="CD9" s="5" t="s">
         <v>123</v>
       </c>
       <c r="CE9" s="1"/>
       <c r="CF9" s="1"/>
-      <c r="CG9" s="55" t="s">
+      <c r="CG9" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="CH9" s="55"/>
-      <c r="CI9" s="55"/>
+      <c r="CH9" s="47"/>
+      <c r="CI9" s="47"/>
       <c r="CM9" s="6" t="s">
         <v>8</v>
       </c>
       <c r="CN9" s="46" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="CO9" s="34"/>
       <c r="CP9" s="34"/>
@@ -8429,7 +8429,7 @@
         <v>8</v>
       </c>
       <c r="AC10" s="46" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AD10" s="34"/>
       <c r="AE10" s="34"/>
@@ -8449,7 +8449,7 @@
         <v>8</v>
       </c>
       <c r="AU10" s="46" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AV10" s="34"/>
       <c r="AW10" s="34"/>
@@ -8459,7 +8459,7 @@
         <v>9</v>
       </c>
       <c r="BD10" s="46" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="BE10" s="34"/>
       <c r="BF10" s="34"/>
@@ -8472,7 +8472,7 @@
       <c r="BP10" s="45"/>
       <c r="BQ10" s="45"/>
       <c r="BU10" s="33" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="BV10" s="33"/>
       <c r="BW10" s="33"/>
@@ -8493,7 +8493,7 @@
         <v>9</v>
       </c>
       <c r="CN10" s="46" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="CO10" s="34"/>
       <c r="CP10" s="34"/>
@@ -8531,7 +8531,7 @@
         <v>9</v>
       </c>
       <c r="AC11" s="46" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AD11" s="34"/>
       <c r="AE11" s="34"/>
@@ -8541,7 +8541,7 @@
         <v>9</v>
       </c>
       <c r="AL11" s="46" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AM11" s="34"/>
       <c r="AN11" s="34"/>
@@ -8551,7 +8551,7 @@
         <v>9</v>
       </c>
       <c r="AU11" s="46" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AV11" s="34"/>
       <c r="AW11" s="34"/>
@@ -8560,8 +8560,8 @@
       <c r="BC11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="BD11" s="53" t="s">
-        <v>255</v>
+      <c r="BD11" s="55" t="s">
+        <v>254</v>
       </c>
       <c r="BE11" s="34"/>
       <c r="BF11" s="34"/>
@@ -8574,7 +8574,7 @@
       <c r="BP11" s="45"/>
       <c r="BQ11" s="45"/>
       <c r="BU11" s="44" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="BV11" s="64"/>
       <c r="BW11" s="64"/>
@@ -8595,7 +8595,7 @@
         <v>7</v>
       </c>
       <c r="CN11" s="20" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="CO11" s="20"/>
       <c r="CP11" s="20"/>
@@ -8606,7 +8606,7 @@
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="55" t="s">
         <v>61</v>
       </c>
       <c r="C12" s="34"/>
@@ -8616,7 +8616,7 @@
       <c r="J12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K12" s="53" t="s">
+      <c r="K12" s="55" t="s">
         <v>79</v>
       </c>
       <c r="L12" s="34"/>
@@ -8632,8 +8632,8 @@
       <c r="AB12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AC12" s="53" t="s">
-        <v>196</v>
+      <c r="AC12" s="55" t="s">
+        <v>195</v>
       </c>
       <c r="AD12" s="34"/>
       <c r="AE12" s="34"/>
@@ -8643,7 +8643,7 @@
         <v>7</v>
       </c>
       <c r="AL12" s="46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AM12" s="34"/>
       <c r="AN12" s="34"/>
@@ -8652,15 +8652,15 @@
       <c r="AT12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AU12" s="53" t="s">
-        <v>232</v>
+      <c r="AU12" s="55" t="s">
+        <v>231</v>
       </c>
       <c r="AV12" s="34"/>
       <c r="AW12" s="34"/>
       <c r="AX12" s="34"/>
       <c r="AY12" s="34"/>
       <c r="BC12" s="35" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="BD12" s="35"/>
       <c r="BE12" s="35"/>
@@ -8668,7 +8668,7 @@
       <c r="BG12" s="35"/>
       <c r="BH12" s="35"/>
       <c r="BL12" s="41" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="BM12" s="41"/>
       <c r="BN12" s="41"/>
@@ -8692,7 +8692,7 @@
       <c r="CH12" s="34"/>
       <c r="CI12" s="34"/>
       <c r="CM12" s="35" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="CN12" s="35"/>
       <c r="CO12" s="35"/>
@@ -8716,7 +8716,7 @@
       <c r="N13" s="35"/>
       <c r="O13" s="35"/>
       <c r="S13" s="33" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="T13" s="33"/>
       <c r="U13" s="33"/>
@@ -8724,7 +8724,7 @@
       <c r="W13" s="33"/>
       <c r="X13" s="33"/>
       <c r="AB13" s="44" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AC13" s="44"/>
       <c r="AD13" s="44"/>
@@ -8732,7 +8732,7 @@
       <c r="AF13" s="44"/>
       <c r="AG13" s="44"/>
       <c r="AK13" s="41" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AL13" s="42"/>
       <c r="AM13" s="42"/>
@@ -8740,7 +8740,7 @@
       <c r="AO13" s="42"/>
       <c r="AP13" s="42"/>
       <c r="AT13" s="33" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AU13" s="33"/>
       <c r="AV13" s="33"/>
@@ -8754,7 +8754,7 @@
       <c r="BG13" s="36"/>
       <c r="BH13" s="36"/>
       <c r="BL13" s="44" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="BM13" s="45"/>
       <c r="BN13" s="45"/>
@@ -8765,7 +8765,7 @@
         <v>8</v>
       </c>
       <c r="BV13" s="46" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="BW13" s="34"/>
       <c r="BX13" s="34"/>
@@ -8809,12 +8809,12 @@
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
-      <c r="AB14" s="54"/>
-      <c r="AC14" s="54"/>
-      <c r="AD14" s="54"/>
-      <c r="AE14" s="54"/>
-      <c r="AF14" s="54"/>
-      <c r="AG14" s="54"/>
+      <c r="AB14" s="56"/>
+      <c r="AC14" s="56"/>
+      <c r="AD14" s="56"/>
+      <c r="AE14" s="56"/>
+      <c r="AF14" s="56"/>
+      <c r="AG14" s="56"/>
       <c r="AK14" s="5" t="s">
         <v>50</v>
       </c>
@@ -8832,7 +8832,7 @@
       <c r="AX14" s="1"/>
       <c r="AY14" s="1"/>
       <c r="BC14" s="33" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="BD14" s="33"/>
       <c r="BE14" s="33"/>
@@ -8849,7 +8849,7 @@
         <v>9</v>
       </c>
       <c r="BV14" s="46" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="BW14" s="34"/>
       <c r="BX14" s="34"/>
@@ -8862,7 +8862,7 @@
       <c r="CH14" s="36"/>
       <c r="CI14" s="36"/>
       <c r="CM14" s="41" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="CN14" s="33"/>
       <c r="CO14" s="33"/>
@@ -8892,13 +8892,13 @@
       </c>
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
-      <c r="V15" s="55" t="s">
+      <c r="V15" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="W15" s="55"/>
-      <c r="X15" s="55"/>
+      <c r="W15" s="47"/>
+      <c r="X15" s="47"/>
       <c r="AB15" s="41" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AC15" s="42"/>
       <c r="AD15" s="42"/>
@@ -8920,11 +8920,11 @@
       </c>
       <c r="AU15" s="1"/>
       <c r="AV15" s="1"/>
-      <c r="AW15" s="55" t="s">
+      <c r="AW15" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="AX15" s="55"/>
-      <c r="AY15" s="55"/>
+      <c r="AX15" s="47"/>
+      <c r="AY15" s="47"/>
       <c r="BC15" s="5" t="s">
         <v>98</v>
       </c>
@@ -8934,7 +8934,7 @@
       <c r="BG15" s="1"/>
       <c r="BH15" s="1"/>
       <c r="BL15" s="41" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="BM15" s="41"/>
       <c r="BN15" s="41"/>
@@ -8945,14 +8945,14 @@
         <v>7</v>
       </c>
       <c r="BV15" s="46" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="BW15" s="34"/>
       <c r="BX15" s="34"/>
       <c r="BY15" s="34"/>
       <c r="BZ15" s="34"/>
       <c r="CD15" s="33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="CE15" s="33"/>
       <c r="CF15" s="33"/>
@@ -8960,7 +8960,7 @@
       <c r="CH15" s="33"/>
       <c r="CI15" s="33"/>
       <c r="CM15" s="44" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="CN15" s="44"/>
       <c r="CO15" s="44"/>
@@ -8974,11 +8974,11 @@
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="55" t="s">
+      <c r="D16" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
       <c r="J16" s="5" t="s">
         <v>50</v>
       </c>
@@ -8991,22 +8991,22 @@
         <v>8</v>
       </c>
       <c r="T16" s="46" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="U16" s="34"/>
       <c r="V16" s="34"/>
       <c r="W16" s="34"/>
       <c r="X16" s="34"/>
-      <c r="AB16" s="51" t="s">
-        <v>188</v>
-      </c>
-      <c r="AC16" s="52"/>
-      <c r="AD16" s="52"/>
-      <c r="AE16" s="52"/>
-      <c r="AF16" s="52"/>
-      <c r="AG16" s="52"/>
+      <c r="AB16" s="53" t="s">
+        <v>187</v>
+      </c>
+      <c r="AC16" s="54"/>
+      <c r="AD16" s="54"/>
+      <c r="AE16" s="54"/>
+      <c r="AF16" s="54"/>
+      <c r="AG16" s="54"/>
       <c r="AK16" s="44" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AL16" s="44"/>
       <c r="AM16" s="44"/>
@@ -9014,7 +9014,7 @@
       <c r="AO16" s="44"/>
       <c r="AP16" s="44"/>
       <c r="AT16" s="45" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AU16" s="45"/>
       <c r="AV16" s="45"/>
@@ -9022,17 +9022,17 @@
       <c r="AX16" s="45"/>
       <c r="AY16" s="45"/>
       <c r="BC16" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="BD16" s="1"/>
       <c r="BE16" s="1"/>
       <c r="BF16" s="18"/>
       <c r="BG16" s="28"/>
       <c r="BH16" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="BL16" s="44" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="BM16" s="45"/>
       <c r="BN16" s="45"/>
@@ -9040,7 +9040,7 @@
       <c r="BP16" s="45"/>
       <c r="BQ16" s="45"/>
       <c r="BU16" s="33" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="BV16" s="33"/>
       <c r="BW16" s="33"/>
@@ -9078,11 +9078,11 @@
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="55" t="s">
+      <c r="M17" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="N17" s="56"/>
-      <c r="O17" s="56"/>
+      <c r="N17" s="48"/>
+      <c r="O17" s="48"/>
       <c r="S17" s="6" t="s">
         <v>9</v>
       </c>
@@ -9093,12 +9093,12 @@
       <c r="V17" s="34"/>
       <c r="W17" s="34"/>
       <c r="X17" s="34"/>
-      <c r="AB17" s="52"/>
-      <c r="AC17" s="52"/>
-      <c r="AD17" s="52"/>
-      <c r="AE17" s="52"/>
-      <c r="AF17" s="52"/>
-      <c r="AG17" s="52"/>
+      <c r="AB17" s="54"/>
+      <c r="AC17" s="54"/>
+      <c r="AD17" s="54"/>
+      <c r="AE17" s="54"/>
+      <c r="AF17" s="54"/>
+      <c r="AG17" s="54"/>
       <c r="AK17" s="44"/>
       <c r="AL17" s="44"/>
       <c r="AM17" s="44"/>
@@ -9112,7 +9112,7 @@
       <c r="AX17" s="45"/>
       <c r="AY17" s="45"/>
       <c r="BC17" s="45" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="BD17" s="45"/>
       <c r="BE17" s="45"/>
@@ -9126,7 +9126,7 @@
       <c r="BP17" s="45"/>
       <c r="BQ17" s="45"/>
       <c r="BU17" s="44" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="BV17" s="44"/>
       <c r="BW17" s="44"/>
@@ -9173,14 +9173,14 @@
         <v>7</v>
       </c>
       <c r="T18" s="46" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="U18" s="34"/>
       <c r="V18" s="34"/>
       <c r="W18" s="34"/>
       <c r="X18" s="34"/>
       <c r="AK18" s="44" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AL18" s="44"/>
       <c r="AM18" s="44"/>
@@ -9200,7 +9200,7 @@
       <c r="BG18" s="45"/>
       <c r="BH18" s="45"/>
       <c r="BL18" s="33" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="BM18" s="33"/>
       <c r="BN18" s="33"/>
@@ -9250,19 +9250,19 @@
       <c r="N19" s="33"/>
       <c r="O19" s="33"/>
       <c r="S19" s="35" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="T19" s="35"/>
       <c r="U19" s="35"/>
       <c r="V19" s="35"/>
       <c r="W19" s="35"/>
       <c r="X19" s="35"/>
-      <c r="AK19" s="54"/>
-      <c r="AL19" s="54"/>
-      <c r="AM19" s="54"/>
-      <c r="AN19" s="54"/>
-      <c r="AO19" s="54"/>
-      <c r="AP19" s="54"/>
+      <c r="AK19" s="56"/>
+      <c r="AL19" s="56"/>
+      <c r="AM19" s="56"/>
+      <c r="AN19" s="56"/>
+      <c r="AO19" s="56"/>
+      <c r="AP19" s="56"/>
       <c r="AT19" s="45"/>
       <c r="AU19" s="45"/>
       <c r="AV19" s="45"/>
@@ -9276,7 +9276,7 @@
       <c r="BG19" s="63"/>
       <c r="BH19" s="63"/>
       <c r="BL19" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="BM19" s="1"/>
       <c r="BN19" s="1"/>
@@ -9300,7 +9300,7 @@
       <c r="CH19" s="34"/>
       <c r="CI19" s="34"/>
       <c r="CM19" s="41" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="CN19" s="33"/>
       <c r="CO19" s="33"/>
@@ -9332,7 +9332,7 @@
       <c r="W20" s="35"/>
       <c r="X20" s="35"/>
       <c r="AK20" s="41" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AL20" s="42"/>
       <c r="AM20" s="42"/>
@@ -9346,7 +9346,7 @@
       <c r="AX20" s="63"/>
       <c r="AY20" s="63"/>
       <c r="BC20" s="41" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BD20" s="42"/>
       <c r="BE20" s="42"/>
@@ -9354,15 +9354,15 @@
       <c r="BG20" s="42"/>
       <c r="BH20" s="42"/>
       <c r="BL20" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="BM20" s="1"/>
       <c r="BN20" s="1"/>
-      <c r="BO20" s="55" t="s">
-        <v>245</v>
-      </c>
-      <c r="BP20" s="55"/>
-      <c r="BQ20" s="55"/>
+      <c r="BO20" s="47" t="s">
+        <v>244</v>
+      </c>
+      <c r="BP20" s="47"/>
+      <c r="BQ20" s="47"/>
       <c r="BU20" s="44"/>
       <c r="BV20" s="44"/>
       <c r="BW20" s="44"/>
@@ -9380,7 +9380,7 @@
       <c r="CH20" s="34"/>
       <c r="CI20" s="34"/>
       <c r="CM20" s="44" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="CN20" s="44"/>
       <c r="CO20" s="44"/>
@@ -9402,46 +9402,46 @@
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-      <c r="M21" s="55" t="s">
+      <c r="M21" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="N21" s="56"/>
-      <c r="O21" s="56"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="48"/>
       <c r="S21" s="36"/>
       <c r="T21" s="36"/>
       <c r="U21" s="36"/>
       <c r="V21" s="36"/>
       <c r="W21" s="36"/>
       <c r="X21" s="36"/>
-      <c r="AK21" s="51" t="s">
-        <v>260</v>
-      </c>
-      <c r="AL21" s="51"/>
-      <c r="AM21" s="51"/>
-      <c r="AN21" s="51"/>
-      <c r="AO21" s="51"/>
-      <c r="AP21" s="51"/>
+      <c r="AK21" s="53" t="s">
+        <v>259</v>
+      </c>
+      <c r="AL21" s="53"/>
+      <c r="AM21" s="53"/>
+      <c r="AN21" s="53"/>
+      <c r="AO21" s="53"/>
+      <c r="AP21" s="53"/>
       <c r="AT21" s="41" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AU21" s="42"/>
       <c r="AV21" s="42"/>
       <c r="AW21" s="42"/>
       <c r="AX21" s="42"/>
       <c r="AY21" s="42"/>
-      <c r="BC21" s="51" t="s">
-        <v>261</v>
-      </c>
-      <c r="BD21" s="51"/>
-      <c r="BE21" s="51"/>
-      <c r="BF21" s="51"/>
-      <c r="BG21" s="51"/>
-      <c r="BH21" s="51"/>
+      <c r="BC21" s="53" t="s">
+        <v>260</v>
+      </c>
+      <c r="BD21" s="53"/>
+      <c r="BE21" s="53"/>
+      <c r="BF21" s="53"/>
+      <c r="BG21" s="53"/>
+      <c r="BH21" s="53"/>
       <c r="BL21" s="6" t="s">
         <v>8</v>
       </c>
       <c r="BM21" s="46" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="BN21" s="46"/>
       <c r="BO21" s="46"/>
@@ -9486,38 +9486,38 @@
       <c r="N22" s="37"/>
       <c r="O22" s="37"/>
       <c r="S22" s="33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="T22" s="33"/>
       <c r="U22" s="33"/>
       <c r="V22" s="33"/>
       <c r="W22" s="33"/>
       <c r="X22" s="33"/>
-      <c r="AK22" s="51"/>
-      <c r="AL22" s="51"/>
-      <c r="AM22" s="51"/>
-      <c r="AN22" s="51"/>
-      <c r="AO22" s="51"/>
-      <c r="AP22" s="51"/>
-      <c r="AT22" s="51" t="s">
-        <v>259</v>
-      </c>
-      <c r="AU22" s="51"/>
-      <c r="AV22" s="51"/>
-      <c r="AW22" s="51"/>
-      <c r="AX22" s="51"/>
-      <c r="AY22" s="51"/>
-      <c r="BC22" s="51"/>
-      <c r="BD22" s="51"/>
-      <c r="BE22" s="51"/>
-      <c r="BF22" s="51"/>
-      <c r="BG22" s="51"/>
-      <c r="BH22" s="51"/>
+      <c r="AK22" s="53"/>
+      <c r="AL22" s="53"/>
+      <c r="AM22" s="53"/>
+      <c r="AN22" s="53"/>
+      <c r="AO22" s="53"/>
+      <c r="AP22" s="53"/>
+      <c r="AT22" s="53" t="s">
+        <v>258</v>
+      </c>
+      <c r="AU22" s="53"/>
+      <c r="AV22" s="53"/>
+      <c r="AW22" s="53"/>
+      <c r="AX22" s="53"/>
+      <c r="AY22" s="53"/>
+      <c r="BC22" s="53"/>
+      <c r="BD22" s="53"/>
+      <c r="BE22" s="53"/>
+      <c r="BF22" s="53"/>
+      <c r="BG22" s="53"/>
+      <c r="BH22" s="53"/>
       <c r="BL22" s="6" t="s">
         <v>9</v>
       </c>
       <c r="BM22" s="46" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="BN22" s="46"/>
       <c r="BO22" s="46"/>
@@ -9550,11 +9550,11 @@
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="55" t="s">
+      <c r="D23" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
       <c r="J23" s="39" t="s">
         <v>84</v>
       </c>
@@ -9571,29 +9571,29 @@
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
-      <c r="AK23" s="51"/>
-      <c r="AL23" s="51"/>
-      <c r="AM23" s="51"/>
-      <c r="AN23" s="51"/>
-      <c r="AO23" s="51"/>
-      <c r="AP23" s="51"/>
-      <c r="AT23" s="51"/>
-      <c r="AU23" s="51"/>
-      <c r="AV23" s="51"/>
-      <c r="AW23" s="51"/>
-      <c r="AX23" s="51"/>
-      <c r="AY23" s="51"/>
-      <c r="BC23" s="51"/>
-      <c r="BD23" s="51"/>
-      <c r="BE23" s="51"/>
-      <c r="BF23" s="51"/>
-      <c r="BG23" s="51"/>
-      <c r="BH23" s="51"/>
+      <c r="AK23" s="53"/>
+      <c r="AL23" s="53"/>
+      <c r="AM23" s="53"/>
+      <c r="AN23" s="53"/>
+      <c r="AO23" s="53"/>
+      <c r="AP23" s="53"/>
+      <c r="AT23" s="53"/>
+      <c r="AU23" s="53"/>
+      <c r="AV23" s="53"/>
+      <c r="AW23" s="53"/>
+      <c r="AX23" s="53"/>
+      <c r="AY23" s="53"/>
+      <c r="BC23" s="53"/>
+      <c r="BD23" s="53"/>
+      <c r="BE23" s="53"/>
+      <c r="BF23" s="53"/>
+      <c r="BG23" s="53"/>
+      <c r="BH23" s="53"/>
       <c r="BL23" s="1" t="s">
         <v>7</v>
       </c>
       <c r="BM23" s="46" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="BN23" s="34"/>
       <c r="BO23" s="34"/>
@@ -9645,14 +9645,14 @@
       <c r="X24" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="AT24" s="51"/>
-      <c r="AU24" s="51"/>
-      <c r="AV24" s="51"/>
-      <c r="AW24" s="51"/>
-      <c r="AX24" s="51"/>
-      <c r="AY24" s="51"/>
+      <c r="AT24" s="53"/>
+      <c r="AU24" s="53"/>
+      <c r="AV24" s="53"/>
+      <c r="AW24" s="53"/>
+      <c r="AX24" s="53"/>
+      <c r="AY24" s="53"/>
       <c r="BC24" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="BD24" s="33"/>
       <c r="BE24" s="33"/>
@@ -9660,7 +9660,7 @@
       <c r="BG24" s="33"/>
       <c r="BH24" s="33"/>
       <c r="BL24" s="36" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="BM24" s="36"/>
       <c r="BN24" s="36"/>
@@ -9691,26 +9691,26 @@
       <c r="D25" s="42"/>
       <c r="E25" s="42"/>
       <c r="F25" s="42"/>
-      <c r="J25" s="52" t="s">
+      <c r="J25" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="K25" s="52"/>
-      <c r="L25" s="52"/>
-      <c r="M25" s="52"/>
-      <c r="N25" s="52"/>
-      <c r="O25" s="52"/>
+      <c r="K25" s="54"/>
+      <c r="L25" s="54"/>
+      <c r="M25" s="54"/>
+      <c r="N25" s="54"/>
+      <c r="O25" s="54"/>
       <c r="S25" s="6" t="s">
         <v>8</v>
       </c>
       <c r="T25" s="46" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="U25" s="34"/>
       <c r="V25" s="34"/>
       <c r="W25" s="34"/>
       <c r="X25" s="34"/>
       <c r="AT25" s="41" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AU25" s="42"/>
       <c r="AV25" s="42"/>
@@ -9718,7 +9718,7 @@
       <c r="AX25" s="42"/>
       <c r="AY25" s="42"/>
       <c r="BC25" s="44" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="BD25" s="44"/>
       <c r="BE25" s="44"/>
@@ -9726,7 +9726,7 @@
       <c r="BG25" s="44"/>
       <c r="BH25" s="44"/>
       <c r="BL25" s="33" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="BM25" s="33"/>
       <c r="BN25" s="33"/>
@@ -9749,38 +9749,38 @@
       <c r="CR25" s="44"/>
     </row>
     <row r="26" spans="1:96" ht="15" customHeight="1">
-      <c r="A26" s="52" t="s">
+      <c r="A26" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="52"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
-      <c r="J26" s="52"/>
-      <c r="K26" s="52"/>
-      <c r="L26" s="52"/>
-      <c r="M26" s="52"/>
-      <c r="N26" s="52"/>
-      <c r="O26" s="52"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="54"/>
+      <c r="L26" s="54"/>
+      <c r="M26" s="54"/>
+      <c r="N26" s="54"/>
+      <c r="O26" s="54"/>
       <c r="S26" s="6" t="s">
         <v>9</v>
       </c>
       <c r="T26" s="46" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="U26" s="34"/>
       <c r="V26" s="34"/>
       <c r="W26" s="34"/>
       <c r="X26" s="34"/>
-      <c r="AT26" s="51" t="s">
-        <v>303</v>
-      </c>
-      <c r="AU26" s="51"/>
-      <c r="AV26" s="51"/>
-      <c r="AW26" s="51"/>
-      <c r="AX26" s="51"/>
-      <c r="AY26" s="51"/>
+      <c r="AT26" s="53" t="s">
+        <v>302</v>
+      </c>
+      <c r="AU26" s="53"/>
+      <c r="AV26" s="53"/>
+      <c r="AW26" s="53"/>
+      <c r="AX26" s="53"/>
+      <c r="AY26" s="53"/>
       <c r="BC26" s="44"/>
       <c r="BD26" s="44"/>
       <c r="BE26" s="44"/>
@@ -9809,40 +9809,40 @@
       <c r="CR26" s="44"/>
     </row>
     <row r="27" spans="1:96">
-      <c r="A27" s="52"/>
-      <c r="B27" s="52"/>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
-      <c r="J27" s="52"/>
-      <c r="K27" s="52"/>
-      <c r="L27" s="52"/>
-      <c r="M27" s="52"/>
-      <c r="N27" s="52"/>
-      <c r="O27" s="52"/>
+      <c r="A27" s="54"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="J27" s="54"/>
+      <c r="K27" s="54"/>
+      <c r="L27" s="54"/>
+      <c r="M27" s="54"/>
+      <c r="N27" s="54"/>
+      <c r="O27" s="54"/>
       <c r="S27" s="1" t="s">
         <v>7</v>
       </c>
       <c r="T27" s="46" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="U27" s="34"/>
       <c r="V27" s="34"/>
       <c r="W27" s="34"/>
       <c r="X27" s="34"/>
-      <c r="AT27" s="51"/>
-      <c r="AU27" s="51"/>
-      <c r="AV27" s="51"/>
-      <c r="AW27" s="51"/>
-      <c r="AX27" s="51"/>
-      <c r="AY27" s="51"/>
-      <c r="BC27" s="54"/>
-      <c r="BD27" s="54"/>
-      <c r="BE27" s="54"/>
-      <c r="BF27" s="54"/>
-      <c r="BG27" s="54"/>
-      <c r="BH27" s="54"/>
+      <c r="AT27" s="53"/>
+      <c r="AU27" s="53"/>
+      <c r="AV27" s="53"/>
+      <c r="AW27" s="53"/>
+      <c r="AX27" s="53"/>
+      <c r="AY27" s="53"/>
+      <c r="BC27" s="56"/>
+      <c r="BD27" s="56"/>
+      <c r="BE27" s="56"/>
+      <c r="BF27" s="56"/>
+      <c r="BG27" s="56"/>
+      <c r="BH27" s="56"/>
       <c r="BL27" s="5" t="s">
         <v>51</v>
       </c>
@@ -9853,12 +9853,12 @@
       <c r="BQ27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="CD27" s="54"/>
-      <c r="CE27" s="54"/>
-      <c r="CF27" s="54"/>
-      <c r="CG27" s="54"/>
-      <c r="CH27" s="54"/>
-      <c r="CI27" s="54"/>
+      <c r="CD27" s="56"/>
+      <c r="CE27" s="56"/>
+      <c r="CF27" s="56"/>
+      <c r="CG27" s="56"/>
+      <c r="CH27" s="56"/>
+      <c r="CI27" s="56"/>
     </row>
     <row r="28" spans="1:96" ht="15" customHeight="1">
       <c r="J28" s="41" t="s">
@@ -9877,14 +9877,14 @@
       <c r="V28" s="42"/>
       <c r="W28" s="42"/>
       <c r="X28" s="42"/>
-      <c r="AT28" s="51"/>
-      <c r="AU28" s="51"/>
-      <c r="AV28" s="51"/>
-      <c r="AW28" s="51"/>
-      <c r="AX28" s="51"/>
-      <c r="AY28" s="51"/>
+      <c r="AT28" s="53"/>
+      <c r="AU28" s="53"/>
+      <c r="AV28" s="53"/>
+      <c r="AW28" s="53"/>
+      <c r="AX28" s="53"/>
+      <c r="AY28" s="53"/>
       <c r="BC28" s="33" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="BD28" s="33"/>
       <c r="BE28" s="33"/>
@@ -9892,7 +9892,7 @@
       <c r="BG28" s="33"/>
       <c r="BH28" s="33"/>
       <c r="BL28" s="44" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="BM28" s="44"/>
       <c r="BN28" s="44"/>
@@ -9954,11 +9954,11 @@
       </c>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
-      <c r="M30" s="55" t="s">
+      <c r="M30" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="N30" s="56"/>
-      <c r="O30" s="56"/>
+      <c r="N30" s="48"/>
+      <c r="O30" s="48"/>
       <c r="S30" s="58"/>
       <c r="T30" s="58"/>
       <c r="U30" s="58"/>
@@ -9966,17 +9966,17 @@
       <c r="W30" s="58"/>
       <c r="X30" s="58"/>
       <c r="BC30" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="BD30" s="1"/>
       <c r="BE30" s="1"/>
-      <c r="BF30" s="55" t="s">
-        <v>250</v>
-      </c>
-      <c r="BG30" s="56"/>
-      <c r="BH30" s="56"/>
+      <c r="BF30" s="47" t="s">
+        <v>249</v>
+      </c>
+      <c r="BG30" s="48"/>
+      <c r="BH30" s="48"/>
       <c r="BL30" s="33" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="BM30" s="33"/>
       <c r="BN30" s="33"/>
@@ -9988,11 +9988,11 @@
       </c>
       <c r="CE30" s="1"/>
       <c r="CF30" s="1"/>
-      <c r="CG30" s="55" t="s">
+      <c r="CG30" s="47" t="s">
         <v>127</v>
       </c>
-      <c r="CH30" s="56"/>
-      <c r="CI30" s="56"/>
+      <c r="CH30" s="48"/>
+      <c r="CI30" s="48"/>
     </row>
     <row r="31" spans="1:96">
       <c r="J31" s="35" t="s">
@@ -10012,7 +10012,7 @@
       <c r="W31" s="33"/>
       <c r="X31" s="33"/>
       <c r="BC31" s="65" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="BD31" s="65"/>
       <c r="BE31" s="65"/>
@@ -10020,7 +10020,7 @@
       <c r="BG31" s="65"/>
       <c r="BH31" s="65"/>
       <c r="BL31" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="BM31" s="1"/>
       <c r="BN31" s="1"/>
@@ -10062,11 +10062,11 @@
       </c>
       <c r="BM32" s="1"/>
       <c r="BN32" s="1"/>
-      <c r="BO32" s="55" t="s">
+      <c r="BO32" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="BP32" s="56"/>
-      <c r="BQ32" s="56"/>
+      <c r="BP32" s="48"/>
+      <c r="BQ32" s="48"/>
       <c r="CD32" s="44" t="s">
         <v>150</v>
       </c>
@@ -10098,7 +10098,7 @@
       <c r="BG33" s="65"/>
       <c r="BH33" s="65"/>
       <c r="BL33" s="37" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="BM33" s="37"/>
       <c r="BN33" s="37"/>
@@ -10121,14 +10121,14 @@
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
-      <c r="S34" s="54"/>
-      <c r="T34" s="54"/>
-      <c r="U34" s="54"/>
-      <c r="V34" s="54"/>
-      <c r="W34" s="54"/>
-      <c r="X34" s="54"/>
+      <c r="S34" s="56"/>
+      <c r="T34" s="56"/>
+      <c r="U34" s="56"/>
+      <c r="V34" s="56"/>
+      <c r="W34" s="56"/>
+      <c r="X34" s="56"/>
       <c r="BC34" s="44" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="BD34" s="44"/>
       <c r="BE34" s="44"/>
@@ -10136,7 +10136,7 @@
       <c r="BG34" s="44"/>
       <c r="BH34" s="44"/>
       <c r="BL34" s="44" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="BM34" s="44"/>
       <c r="BN34" s="44"/>
@@ -10156,11 +10156,11 @@
       </c>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
-      <c r="M35" s="55" t="s">
+      <c r="M35" s="47" t="s">
         <v>100</v>
       </c>
-      <c r="N35" s="56"/>
-      <c r="O35" s="56"/>
+      <c r="N35" s="48"/>
+      <c r="O35" s="48"/>
       <c r="S35" s="33" t="s">
         <v>141</v>
       </c>
@@ -10236,13 +10236,13 @@
       </c>
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
-      <c r="V37" s="55" t="s">
+      <c r="V37" s="47" t="s">
         <v>127</v>
       </c>
-      <c r="W37" s="56"/>
-      <c r="X37" s="56"/>
+      <c r="W37" s="48"/>
+      <c r="X37" s="48"/>
       <c r="BC37" s="33" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="BD37" s="33"/>
       <c r="BE37" s="33"/>
@@ -10302,11 +10302,11 @@
       </c>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
-      <c r="M39" s="55" t="s">
+      <c r="M39" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="N39" s="56"/>
-      <c r="O39" s="56"/>
+      <c r="N39" s="48"/>
+      <c r="O39" s="48"/>
       <c r="S39" s="44" t="s">
         <v>150</v>
       </c>
@@ -10320,11 +10320,11 @@
       </c>
       <c r="BD39" s="1"/>
       <c r="BE39" s="1"/>
-      <c r="BF39" s="55" t="s">
+      <c r="BF39" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="BG39" s="56"/>
-      <c r="BH39" s="56"/>
+      <c r="BG39" s="48"/>
+      <c r="BH39" s="48"/>
       <c r="CD39" s="44" t="s">
         <v>139</v>
       </c>
@@ -10350,7 +10350,7 @@
       <c r="W40" s="44"/>
       <c r="X40" s="44"/>
       <c r="BC40" s="37" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="BD40" s="37"/>
       <c r="BE40" s="37"/>
@@ -10372,7 +10372,7 @@
       <c r="W41" s="44"/>
       <c r="X41" s="44"/>
       <c r="BC41" s="44" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="BD41" s="44"/>
       <c r="BE41" s="44"/>
@@ -10454,7 +10454,7 @@
     </row>
     <row r="48" spans="10:87">
       <c r="BC48" s="41" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="BD48" s="41"/>
       <c r="BE48" s="41"/>
@@ -10462,7 +10462,7 @@
       <c r="BG48" s="41"/>
       <c r="BH48" s="41"/>
       <c r="CD48" s="41" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="CE48" s="42"/>
       <c r="CF48" s="42"/>
@@ -10472,7 +10472,7 @@
     </row>
     <row r="49" spans="55:87">
       <c r="BC49" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="BD49" s="1"/>
       <c r="BE49" s="1"/>
@@ -10494,25 +10494,25 @@
       </c>
       <c r="BD50" s="1"/>
       <c r="BE50" s="1"/>
-      <c r="BF50" s="55" t="s">
-        <v>277</v>
-      </c>
-      <c r="BG50" s="55"/>
-      <c r="BH50" s="55"/>
+      <c r="BF50" s="47" t="s">
+        <v>276</v>
+      </c>
+      <c r="BG50" s="47"/>
+      <c r="BH50" s="47"/>
       <c r="CD50" s="5" t="s">
         <v>94</v>
       </c>
       <c r="CE50" s="1"/>
       <c r="CF50" s="1"/>
-      <c r="CG50" s="55" t="s">
+      <c r="CG50" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="CH50" s="56"/>
-      <c r="CI50" s="56"/>
+      <c r="CH50" s="48"/>
+      <c r="CI50" s="48"/>
     </row>
     <row r="51" spans="55:87" ht="15" customHeight="1">
       <c r="BC51" s="35" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="BD51" s="35"/>
       <c r="BE51" s="35"/>
@@ -10520,7 +10520,7 @@
       <c r="BG51" s="35"/>
       <c r="BH51" s="35"/>
       <c r="BL51" s="41" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="BM51" s="41"/>
       <c r="BN51" s="41"/>
@@ -10560,7 +10560,7 @@
     </row>
     <row r="53" spans="55:87">
       <c r="BC53" s="41" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="BD53" s="41"/>
       <c r="BE53" s="41"/>
@@ -10568,14 +10568,14 @@
       <c r="BG53" s="41"/>
       <c r="BH53" s="41"/>
       <c r="BL53" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="BM53" s="1"/>
       <c r="BN53" s="1"/>
       <c r="BO53" s="18"/>
       <c r="BP53" s="18"/>
       <c r="BQ53" s="18" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="CD53" s="41" t="s">
         <v>97</v>
@@ -10596,7 +10596,7 @@
       <c r="BG54" s="1"/>
       <c r="BH54" s="1"/>
       <c r="BL54" s="35" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="BM54" s="35"/>
       <c r="BN54" s="35"/>
@@ -10614,20 +10614,20 @@
     </row>
     <row r="55" spans="55:87" ht="15" customHeight="1">
       <c r="BC55" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="BD55" s="1"/>
       <c r="BE55" s="1"/>
-      <c r="BF55" s="55" t="s">
+      <c r="BF55" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="BG55" s="55"/>
-      <c r="BH55" s="55"/>
+      <c r="BG55" s="47"/>
+      <c r="BH55" s="47"/>
       <c r="BL55" s="6" t="s">
         <v>8</v>
       </c>
       <c r="BM55" s="46" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="BN55" s="34"/>
       <c r="BO55" s="34"/>
@@ -10638,15 +10638,15 @@
       </c>
       <c r="CE55" s="1"/>
       <c r="CF55" s="1"/>
-      <c r="CG55" s="55" t="s">
+      <c r="CG55" s="47" t="s">
         <v>100</v>
       </c>
-      <c r="CH55" s="56"/>
-      <c r="CI55" s="56"/>
+      <c r="CH55" s="48"/>
+      <c r="CI55" s="48"/>
     </row>
     <row r="56" spans="55:87">
       <c r="BC56" s="35" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="BD56" s="35"/>
       <c r="BE56" s="35"/>
@@ -10657,7 +10657,7 @@
         <v>9</v>
       </c>
       <c r="BM56" s="46" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="BN56" s="34"/>
       <c r="BO56" s="34"/>
@@ -10683,7 +10683,7 @@
         <v>7</v>
       </c>
       <c r="BM57" s="20" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="BN57" s="7"/>
       <c r="BO57" s="7"/>
@@ -10700,7 +10700,7 @@
     </row>
     <row r="58" spans="55:87" ht="15" customHeight="1">
       <c r="BC58" s="41" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="BD58" s="41"/>
       <c r="BE58" s="41"/>
@@ -10708,7 +10708,7 @@
       <c r="BG58" s="41"/>
       <c r="BH58" s="41"/>
       <c r="BL58" s="41" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="BM58" s="41"/>
       <c r="BN58" s="41"/>
@@ -10734,7 +10734,7 @@
       <c r="BG59" s="1"/>
       <c r="BH59" s="1"/>
       <c r="BL59" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="BM59" s="1"/>
       <c r="BN59" s="1"/>
@@ -10746,11 +10746,11 @@
       </c>
       <c r="CE59" s="1"/>
       <c r="CF59" s="1"/>
-      <c r="CG59" s="55" t="s">
+      <c r="CG59" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="CH59" s="56"/>
-      <c r="CI59" s="56"/>
+      <c r="CH59" s="48"/>
+      <c r="CI59" s="48"/>
     </row>
     <row r="60" spans="55:87" ht="15" customHeight="1">
       <c r="BC60" s="5" t="s">
@@ -10758,21 +10758,21 @@
       </c>
       <c r="BD60" s="1"/>
       <c r="BE60" s="1"/>
-      <c r="BF60" s="55" t="s">
+      <c r="BF60" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="BG60" s="56"/>
-      <c r="BH60" s="56"/>
+      <c r="BG60" s="48"/>
+      <c r="BH60" s="48"/>
       <c r="BL60" s="5" t="s">
         <v>51</v>
       </c>
       <c r="BM60" s="1"/>
       <c r="BN60" s="1"/>
-      <c r="BO60" s="55" t="s">
+      <c r="BO60" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="BP60" s="55"/>
-      <c r="BQ60" s="55"/>
+      <c r="BP60" s="47"/>
+      <c r="BQ60" s="47"/>
       <c r="CD60" s="35" t="s">
         <v>106</v>
       </c>
@@ -10784,7 +10784,7 @@
     </row>
     <row r="61" spans="55:87">
       <c r="BC61" s="35" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="BD61" s="35"/>
       <c r="BE61" s="35"/>
@@ -10792,7 +10792,7 @@
       <c r="BG61" s="35"/>
       <c r="BH61" s="35"/>
       <c r="BL61" s="35" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="BM61" s="35"/>
       <c r="BN61" s="35"/>
@@ -10842,7 +10842,7 @@
     </row>
     <row r="64" spans="55:87" ht="15" customHeight="1">
       <c r="BL64" s="41" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="BM64" s="41"/>
       <c r="BN64" s="41"/>
@@ -10866,15 +10866,15 @@
       </c>
       <c r="BM66" s="1"/>
       <c r="BN66" s="1"/>
-      <c r="BO66" s="55" t="s">
+      <c r="BO66" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="BP66" s="56"/>
-      <c r="BQ66" s="56"/>
+      <c r="BP66" s="48"/>
+      <c r="BQ66" s="48"/>
     </row>
     <row r="67" spans="64:69">
       <c r="BL67" s="35" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="BM67" s="35"/>
       <c r="BN67" s="35"/>
@@ -10938,6 +10938,8 @@
     <mergeCell ref="BF30:BH30"/>
     <mergeCell ref="BC31:BH33"/>
     <mergeCell ref="BC34:BH36"/>
+    <mergeCell ref="BL5:BQ5"/>
+    <mergeCell ref="BL6:BQ6"/>
     <mergeCell ref="BU2:BZ3"/>
     <mergeCell ref="BU16:BZ16"/>
     <mergeCell ref="BU11:BZ12"/>
@@ -10949,8 +10951,6 @@
     <mergeCell ref="BU10:BZ10"/>
     <mergeCell ref="BV14:BZ14"/>
     <mergeCell ref="BV15:BZ15"/>
-    <mergeCell ref="BL5:BQ5"/>
-    <mergeCell ref="BL6:BQ6"/>
     <mergeCell ref="BL7:BQ8"/>
     <mergeCell ref="BL18:BQ18"/>
     <mergeCell ref="BL30:BQ30"/>
@@ -10960,6 +10960,21 @@
     <mergeCell ref="CD60:CI62"/>
     <mergeCell ref="BF60:BH60"/>
     <mergeCell ref="BC61:BH63"/>
+    <mergeCell ref="CE20:CI20"/>
+    <mergeCell ref="CD21:CI21"/>
+    <mergeCell ref="CD22:CI23"/>
+    <mergeCell ref="CD24:CI24"/>
+    <mergeCell ref="CD48:CI48"/>
+    <mergeCell ref="CG50:CI50"/>
+    <mergeCell ref="CD51:CI52"/>
+    <mergeCell ref="CD53:CI53"/>
+    <mergeCell ref="CG55:CI55"/>
+    <mergeCell ref="CE36:CI36"/>
+    <mergeCell ref="CE37:CI37"/>
+    <mergeCell ref="CD39:CI39"/>
+    <mergeCell ref="CD25:CI27"/>
+    <mergeCell ref="CD28:CI28"/>
+    <mergeCell ref="CG30:CI30"/>
     <mergeCell ref="AT13:AY13"/>
     <mergeCell ref="AW15:AY15"/>
     <mergeCell ref="AT16:AY20"/>
@@ -10978,21 +10993,6 @@
     <mergeCell ref="BC40:BH40"/>
     <mergeCell ref="BC24:BH24"/>
     <mergeCell ref="BC28:BH28"/>
-    <mergeCell ref="CE20:CI20"/>
-    <mergeCell ref="CD21:CI21"/>
-    <mergeCell ref="CD22:CI23"/>
-    <mergeCell ref="CD24:CI24"/>
-    <mergeCell ref="CD48:CI48"/>
-    <mergeCell ref="CG50:CI50"/>
-    <mergeCell ref="CD51:CI52"/>
-    <mergeCell ref="CD53:CI53"/>
-    <mergeCell ref="CG55:CI55"/>
-    <mergeCell ref="CE36:CI36"/>
-    <mergeCell ref="CE37:CI37"/>
-    <mergeCell ref="CD39:CI39"/>
-    <mergeCell ref="CD25:CI27"/>
-    <mergeCell ref="CD28:CI28"/>
-    <mergeCell ref="CG30:CI30"/>
     <mergeCell ref="CD31:CI31"/>
     <mergeCell ref="CD32:CI35"/>
     <mergeCell ref="CD6:CI6"/>
@@ -11029,22 +11029,6 @@
     <mergeCell ref="AK5:AN5"/>
     <mergeCell ref="AK20:AP20"/>
     <mergeCell ref="AK6:AP6"/>
-    <mergeCell ref="J18:O18"/>
-    <mergeCell ref="J22:O22"/>
-    <mergeCell ref="J28:O28"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="J23:O23"/>
-    <mergeCell ref="J24:O24"/>
-    <mergeCell ref="J13:O14"/>
-    <mergeCell ref="J19:O19"/>
-    <mergeCell ref="T26:X26"/>
-    <mergeCell ref="T27:X27"/>
-    <mergeCell ref="S13:X13"/>
-    <mergeCell ref="V15:X15"/>
-    <mergeCell ref="T16:X16"/>
-    <mergeCell ref="T17:X17"/>
-    <mergeCell ref="T18:X18"/>
-    <mergeCell ref="S22:X22"/>
     <mergeCell ref="AK7:AP7"/>
     <mergeCell ref="AL10:AP10"/>
     <mergeCell ref="AL11:AP11"/>
@@ -11059,6 +11043,16 @@
     <mergeCell ref="J31:O32"/>
     <mergeCell ref="J33:O33"/>
     <mergeCell ref="J25:O27"/>
+    <mergeCell ref="J18:O18"/>
+    <mergeCell ref="J22:O22"/>
+    <mergeCell ref="J28:O28"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="J23:O23"/>
+    <mergeCell ref="J24:O24"/>
+    <mergeCell ref="J13:O14"/>
+    <mergeCell ref="J19:O19"/>
+    <mergeCell ref="T26:X26"/>
+    <mergeCell ref="T27:X27"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="J6:O6"/>
@@ -11117,6 +11111,12 @@
     <mergeCell ref="AC11:AG11"/>
     <mergeCell ref="AC12:AG12"/>
     <mergeCell ref="AB13:AG14"/>
+    <mergeCell ref="S13:X13"/>
+    <mergeCell ref="V15:X15"/>
+    <mergeCell ref="T16:X16"/>
+    <mergeCell ref="T17:X17"/>
+    <mergeCell ref="T18:X18"/>
+    <mergeCell ref="S22:X22"/>
     <mergeCell ref="BL67:BQ71"/>
     <mergeCell ref="BL12:BQ12"/>
     <mergeCell ref="BL13:BQ14"/>
@@ -11146,8 +11146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02DFD280-CB3F-4A45-8F62-9CF1F8B27A7E}">
   <dimension ref="A1:AP24"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AJ23" sqref="AJ23"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AI17" sqref="AI17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11198,7 +11198,7 @@
       <c r="AF1" s="69"/>
       <c r="AG1" s="69"/>
       <c r="AK1" s="72" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AL1" s="72"/>
       <c r="AM1" s="72"/>
@@ -11218,7 +11218,7 @@
         <v>37</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -11248,7 +11248,7 @@
         <v>37</v>
       </c>
       <c r="AK2" s="21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AL2" s="2"/>
       <c r="AM2" s="2"/>
@@ -11300,13 +11300,13 @@
       </c>
       <c r="AG3" s="66"/>
       <c r="AK3" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AL3" s="1"/>
       <c r="AM3" s="5"/>
       <c r="AN3" s="1"/>
       <c r="AO3" s="66" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AP3" s="66"/>
     </row>
@@ -11352,7 +11352,7 @@
       </c>
       <c r="AG4" s="37"/>
       <c r="AK4" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AL4" s="1"/>
       <c r="AM4" s="1"/>
@@ -11378,7 +11378,7 @@
       <c r="N5" s="32"/>
       <c r="O5" s="32"/>
       <c r="S5" s="31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="T5" s="32"/>
       <c r="U5" s="32"/>
@@ -11394,7 +11394,7 @@
       <c r="AF5" s="32"/>
       <c r="AG5" s="32"/>
       <c r="AK5" s="31" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AL5" s="32"/>
       <c r="AM5" s="32"/>
@@ -11436,7 +11436,7 @@
       <c r="AF6" s="33"/>
       <c r="AG6" s="33"/>
       <c r="AK6" s="41" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AL6" s="41"/>
       <c r="AM6" s="41"/>
@@ -11477,14 +11477,14 @@
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
       <c r="AG7" s="1"/>
-      <c r="AK7" s="51" t="s">
-        <v>177</v>
-      </c>
-      <c r="AL7" s="51"/>
-      <c r="AM7" s="51"/>
-      <c r="AN7" s="51"/>
-      <c r="AO7" s="51"/>
-      <c r="AP7" s="51"/>
+      <c r="AK7" s="53" t="s">
+        <v>176</v>
+      </c>
+      <c r="AL7" s="53"/>
+      <c r="AM7" s="53"/>
+      <c r="AN7" s="53"/>
+      <c r="AO7" s="53"/>
+      <c r="AP7" s="53"/>
     </row>
     <row r="8" spans="1:42">
       <c r="A8" s="5" t="s">
@@ -11500,37 +11500,37 @@
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-      <c r="M8" s="55" t="s">
+      <c r="M8" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="N8" s="55"/>
-      <c r="O8" s="55"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="47"/>
       <c r="S8" s="5" t="s">
         <v>44</v>
       </c>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
-      <c r="V8" s="55" t="s">
+      <c r="V8" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="W8" s="55"/>
-      <c r="X8" s="55"/>
+      <c r="W8" s="47"/>
+      <c r="X8" s="47"/>
       <c r="AB8" s="5" t="s">
         <v>44</v>
       </c>
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
-      <c r="AE8" s="55" t="s">
+      <c r="AE8" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="AF8" s="55"/>
-      <c r="AG8" s="55"/>
-      <c r="AK8" s="51"/>
-      <c r="AL8" s="51"/>
-      <c r="AM8" s="51"/>
-      <c r="AN8" s="51"/>
-      <c r="AO8" s="51"/>
-      <c r="AP8" s="51"/>
+      <c r="AF8" s="47"/>
+      <c r="AG8" s="47"/>
+      <c r="AK8" s="53"/>
+      <c r="AL8" s="53"/>
+      <c r="AM8" s="53"/>
+      <c r="AN8" s="53"/>
+      <c r="AO8" s="53"/>
+      <c r="AP8" s="53"/>
     </row>
     <row r="9" spans="1:42">
       <c r="A9" s="5" t="s">
@@ -11538,11 +11538,11 @@
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="55" t="s">
+      <c r="D9" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
       <c r="J9" s="6" t="s">
         <v>8</v>
       </c>
@@ -11564,19 +11564,19 @@
       <c r="W9" s="34"/>
       <c r="X9" s="34"/>
       <c r="AB9" s="35" t="s">
-        <v>170</v>
-      </c>
-      <c r="AC9" s="52"/>
-      <c r="AD9" s="52"/>
-      <c r="AE9" s="52"/>
-      <c r="AF9" s="52"/>
-      <c r="AG9" s="52"/>
-      <c r="AK9" s="51"/>
-      <c r="AL9" s="51"/>
-      <c r="AM9" s="51"/>
-      <c r="AN9" s="51"/>
-      <c r="AO9" s="51"/>
-      <c r="AP9" s="51"/>
+        <v>347</v>
+      </c>
+      <c r="AC9" s="54"/>
+      <c r="AD9" s="54"/>
+      <c r="AE9" s="54"/>
+      <c r="AF9" s="54"/>
+      <c r="AG9" s="54"/>
+      <c r="AK9" s="53"/>
+      <c r="AL9" s="53"/>
+      <c r="AM9" s="53"/>
+      <c r="AN9" s="53"/>
+      <c r="AO9" s="53"/>
+      <c r="AP9" s="53"/>
     </row>
     <row r="10" spans="1:42" ht="15" customHeight="1">
       <c r="A10" s="6" t="s">
@@ -11609,18 +11609,18 @@
       <c r="V10" s="34"/>
       <c r="W10" s="34"/>
       <c r="X10" s="34"/>
-      <c r="AB10" s="52"/>
-      <c r="AC10" s="52"/>
-      <c r="AD10" s="52"/>
-      <c r="AE10" s="52"/>
-      <c r="AF10" s="52"/>
-      <c r="AG10" s="52"/>
-      <c r="AK10" s="51"/>
-      <c r="AL10" s="51"/>
-      <c r="AM10" s="51"/>
-      <c r="AN10" s="51"/>
-      <c r="AO10" s="51"/>
-      <c r="AP10" s="51"/>
+      <c r="AB10" s="54"/>
+      <c r="AC10" s="54"/>
+      <c r="AD10" s="54"/>
+      <c r="AE10" s="54"/>
+      <c r="AF10" s="54"/>
+      <c r="AG10" s="54"/>
+      <c r="AK10" s="53"/>
+      <c r="AL10" s="53"/>
+      <c r="AM10" s="53"/>
+      <c r="AN10" s="53"/>
+      <c r="AO10" s="53"/>
+      <c r="AP10" s="53"/>
     </row>
     <row r="11" spans="1:42">
       <c r="A11" s="6" t="s">
@@ -11668,7 +11668,7 @@
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="55" t="s">
         <v>61</v>
       </c>
       <c r="C12" s="34"/>
@@ -11715,14 +11715,14 @@
       <c r="M13" s="71"/>
       <c r="N13" s="71"/>
       <c r="O13" s="71"/>
-      <c r="S13" s="52" t="s">
+      <c r="S13" s="54" t="s">
         <v>157</v>
       </c>
-      <c r="T13" s="52"/>
-      <c r="U13" s="52"/>
-      <c r="V13" s="52"/>
-      <c r="W13" s="52"/>
-      <c r="X13" s="52"/>
+      <c r="T13" s="54"/>
+      <c r="U13" s="54"/>
+      <c r="V13" s="54"/>
+      <c r="W13" s="54"/>
+      <c r="X13" s="54"/>
       <c r="AB13" s="1" t="s">
         <v>7</v>
       </c>
@@ -11751,12 +11751,12 @@
       <c r="M14" s="41"/>
       <c r="N14" s="41"/>
       <c r="O14" s="41"/>
-      <c r="S14" s="52"/>
-      <c r="T14" s="52"/>
-      <c r="U14" s="52"/>
-      <c r="V14" s="52"/>
-      <c r="W14" s="52"/>
-      <c r="X14" s="52"/>
+      <c r="S14" s="54"/>
+      <c r="T14" s="54"/>
+      <c r="U14" s="54"/>
+      <c r="V14" s="54"/>
+      <c r="W14" s="54"/>
+      <c r="X14" s="54"/>
       <c r="AB14" s="41" t="s">
         <v>111</v>
       </c>
@@ -11775,14 +11775,14 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="J15" s="52" t="s">
+      <c r="J15" s="54" t="s">
         <v>156</v>
       </c>
-      <c r="K15" s="52"/>
-      <c r="L15" s="52"/>
-      <c r="M15" s="52"/>
-      <c r="N15" s="52"/>
-      <c r="O15" s="52"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="54"/>
+      <c r="N15" s="54"/>
+      <c r="O15" s="54"/>
       <c r="S15" s="41" t="s">
         <v>116</v>
       </c>
@@ -11791,14 +11791,14 @@
       <c r="V15" s="42"/>
       <c r="W15" s="42"/>
       <c r="X15" s="42"/>
-      <c r="AB15" s="52" t="s">
-        <v>306</v>
-      </c>
-      <c r="AC15" s="52"/>
-      <c r="AD15" s="52"/>
-      <c r="AE15" s="52"/>
-      <c r="AF15" s="52"/>
-      <c r="AG15" s="52"/>
+      <c r="AB15" s="54" t="s">
+        <v>305</v>
+      </c>
+      <c r="AC15" s="54"/>
+      <c r="AD15" s="54"/>
+      <c r="AE15" s="54"/>
+      <c r="AF15" s="54"/>
+      <c r="AG15" s="54"/>
     </row>
     <row r="16" spans="1:42">
       <c r="A16" s="5" t="s">
@@ -11806,31 +11806,31 @@
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="55" t="s">
+      <c r="D16" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="J16" s="52"/>
-      <c r="K16" s="52"/>
-      <c r="L16" s="52"/>
-      <c r="M16" s="52"/>
-      <c r="N16" s="52"/>
-      <c r="O16" s="52"/>
-      <c r="S16" s="52" t="s">
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="54"/>
+      <c r="N16" s="54"/>
+      <c r="O16" s="54"/>
+      <c r="S16" s="54" t="s">
         <v>117</v>
       </c>
-      <c r="T16" s="52"/>
-      <c r="U16" s="52"/>
-      <c r="V16" s="52"/>
-      <c r="W16" s="52"/>
-      <c r="X16" s="52"/>
-      <c r="AB16" s="52"/>
-      <c r="AC16" s="52"/>
-      <c r="AD16" s="52"/>
-      <c r="AE16" s="52"/>
-      <c r="AF16" s="52"/>
-      <c r="AG16" s="52"/>
+      <c r="T16" s="54"/>
+      <c r="U16" s="54"/>
+      <c r="V16" s="54"/>
+      <c r="W16" s="54"/>
+      <c r="X16" s="54"/>
+      <c r="AB16" s="54"/>
+      <c r="AC16" s="54"/>
+      <c r="AD16" s="54"/>
+      <c r="AE16" s="54"/>
+      <c r="AF16" s="54"/>
+      <c r="AG16" s="54"/>
     </row>
     <row r="17" spans="1:33" ht="15" customHeight="1">
       <c r="A17" s="6" t="s">
@@ -11843,14 +11843,14 @@
       <c r="D17" s="34"/>
       <c r="E17" s="34"/>
       <c r="F17" s="34"/>
-      <c r="S17" s="52"/>
-      <c r="T17" s="52"/>
-      <c r="U17" s="52"/>
-      <c r="V17" s="52"/>
-      <c r="W17" s="52"/>
-      <c r="X17" s="52"/>
+      <c r="S17" s="54"/>
+      <c r="T17" s="54"/>
+      <c r="U17" s="54"/>
+      <c r="V17" s="54"/>
+      <c r="W17" s="54"/>
+      <c r="X17" s="54"/>
       <c r="AB17" s="41" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AC17" s="41"/>
       <c r="AD17" s="41"/>
@@ -11869,20 +11869,20 @@
       <c r="D18" s="34"/>
       <c r="E18" s="34"/>
       <c r="F18" s="34"/>
-      <c r="S18" s="52"/>
-      <c r="T18" s="52"/>
-      <c r="U18" s="52"/>
-      <c r="V18" s="52"/>
-      <c r="W18" s="52"/>
-      <c r="X18" s="52"/>
-      <c r="AB18" s="51" t="s">
-        <v>305</v>
-      </c>
-      <c r="AC18" s="51"/>
-      <c r="AD18" s="51"/>
-      <c r="AE18" s="51"/>
-      <c r="AF18" s="51"/>
-      <c r="AG18" s="51"/>
+      <c r="S18" s="54"/>
+      <c r="T18" s="54"/>
+      <c r="U18" s="54"/>
+      <c r="V18" s="54"/>
+      <c r="W18" s="54"/>
+      <c r="X18" s="54"/>
+      <c r="AB18" s="53" t="s">
+        <v>304</v>
+      </c>
+      <c r="AC18" s="53"/>
+      <c r="AD18" s="53"/>
+      <c r="AE18" s="53"/>
+      <c r="AF18" s="53"/>
+      <c r="AG18" s="53"/>
     </row>
     <row r="19" spans="1:33">
       <c r="A19" s="1" t="s">
@@ -11895,12 +11895,12 @@
       <c r="D19" s="34"/>
       <c r="E19" s="34"/>
       <c r="F19" s="34"/>
-      <c r="AB19" s="51"/>
-      <c r="AC19" s="51"/>
-      <c r="AD19" s="51"/>
-      <c r="AE19" s="51"/>
-      <c r="AF19" s="51"/>
-      <c r="AG19" s="51"/>
+      <c r="AB19" s="53"/>
+      <c r="AC19" s="53"/>
+      <c r="AD19" s="53"/>
+      <c r="AE19" s="53"/>
+      <c r="AF19" s="53"/>
+      <c r="AG19" s="53"/>
     </row>
     <row r="20" spans="1:33" ht="15" customHeight="1">
       <c r="A20" s="59" t="s">
@@ -11911,12 +11911,12 @@
       <c r="D20" s="59"/>
       <c r="E20" s="59"/>
       <c r="F20" s="59"/>
-      <c r="AB20" s="51"/>
-      <c r="AC20" s="51"/>
-      <c r="AD20" s="51"/>
-      <c r="AE20" s="51"/>
-      <c r="AF20" s="51"/>
-      <c r="AG20" s="51"/>
+      <c r="AB20" s="53"/>
+      <c r="AC20" s="53"/>
+      <c r="AD20" s="53"/>
+      <c r="AE20" s="53"/>
+      <c r="AF20" s="53"/>
+      <c r="AG20" s="53"/>
     </row>
     <row r="21" spans="1:33">
       <c r="A21" s="41" t="s">
@@ -11928,7 +11928,7 @@
       <c r="E21" s="42"/>
       <c r="F21" s="42"/>
       <c r="AB21" s="41" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AC21" s="41"/>
       <c r="AD21" s="41"/>
@@ -11937,44 +11937,44 @@
       <c r="AG21" s="41"/>
     </row>
     <row r="22" spans="1:33" ht="15" customHeight="1">
-      <c r="A22" s="52" t="s">
+      <c r="A22" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="52"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
-      <c r="AB22" s="51" t="s">
-        <v>307</v>
-      </c>
-      <c r="AC22" s="51"/>
-      <c r="AD22" s="51"/>
-      <c r="AE22" s="51"/>
-      <c r="AF22" s="51"/>
-      <c r="AG22" s="51"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
+      <c r="AB22" s="53" t="s">
+        <v>306</v>
+      </c>
+      <c r="AC22" s="53"/>
+      <c r="AD22" s="53"/>
+      <c r="AE22" s="53"/>
+      <c r="AF22" s="53"/>
+      <c r="AG22" s="53"/>
     </row>
     <row r="23" spans="1:33">
-      <c r="A23" s="52"/>
-      <c r="B23" s="52"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="AB23" s="51"/>
-      <c r="AC23" s="51"/>
-      <c r="AD23" s="51"/>
-      <c r="AE23" s="51"/>
-      <c r="AF23" s="51"/>
-      <c r="AG23" s="51"/>
+      <c r="A23" s="54"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="AB23" s="53"/>
+      <c r="AC23" s="53"/>
+      <c r="AD23" s="53"/>
+      <c r="AE23" s="53"/>
+      <c r="AF23" s="53"/>
+      <c r="AG23" s="53"/>
     </row>
     <row r="24" spans="1:33">
-      <c r="AB24" s="51"/>
-      <c r="AC24" s="51"/>
-      <c r="AD24" s="51"/>
-      <c r="AE24" s="51"/>
-      <c r="AF24" s="51"/>
-      <c r="AG24" s="51"/>
+      <c r="AB24" s="53"/>
+      <c r="AC24" s="53"/>
+      <c r="AD24" s="53"/>
+      <c r="AE24" s="53"/>
+      <c r="AF24" s="53"/>
+      <c r="AG24" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="67">
@@ -12048,6 +12048,6 @@
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>